<commit_message>
update generated data Triggered by 0010109da9a048b0d6e11148a0321cd91f9c4d42
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G303"/>
+  <dimension ref="A1:G302"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6524,56 +6524,56 @@
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>PAP</t>
+          <t>UIO</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Port-Au-Prince, Haiti</t>
+          <t>Quito, Ecuador</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>18.5799999237</v>
+        <v>-0.1291666667</v>
       </c>
       <c r="D197" t="n">
-        <v>-72.2925033569</v>
+        <v>-78.3575</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>HT</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Port-au-Prince</t>
+          <t>Quito</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>UIO</t>
+          <t>REC</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Quito, Ecuador</t>
+          <t>Recife, Brazil</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>-0.1291666667</v>
+        <v>-8.126489639300001</v>
       </c>
       <c r="D198" t="n">
-        <v>-78.3575</v>
+        <v>-34.9235992432</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -6583,26 +6583,26 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>Quito</t>
+          <t>Recife</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Recife, Brazil</t>
+          <t>Ribeirao Preto, Brazil</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>-8.126489639300001</v>
+        <v>-21.1363887787</v>
       </c>
       <c r="D199" t="n">
-        <v>-34.9235992432</v>
+        <v>-47.7766685486</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -6616,26 +6616,26 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>Ribeirao Preto</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>GIG</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Ribeirao Preto, Brazil</t>
+          <t>Rio de Janeiro, Brazil</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>-21.1363887787</v>
+        <v>-22.8099994659</v>
       </c>
       <c r="D200" t="n">
-        <v>-47.7766685486</v>
+        <v>-43.2505569458</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -6649,26 +6649,26 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Ribeirao Preto</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>GIG</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Rio de Janeiro, Brazil</t>
+          <t>Salvador, Brazil</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>-22.8099994659</v>
+        <v>-12.9086112976</v>
       </c>
       <c r="D201" t="n">
-        <v>-43.2505569458</v>
+        <v>-38.3224983215</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -6682,30 +6682,30 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Salvador, Brazil</t>
+          <t>San José, Costa Rica</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>-12.9086112976</v>
+        <v>9.9938602448</v>
       </c>
       <c r="D202" t="n">
-        <v>-38.3224983215</v>
+        <v>-84.2088012695</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -6715,30 +6715,30 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>Salvador</t>
+          <t>San José</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>San José, Costa Rica</t>
+          <t>Santiago, Chile</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>9.9938602448</v>
+        <v>-33.3930015564</v>
       </c>
       <c r="D203" t="n">
-        <v>-84.2088012695</v>
+        <v>-70.7857971191</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -6748,92 +6748,92 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Santiago</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SDQ</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Santiago, Chile</t>
+          <t>Santo Domingo, Dominican Republic</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>-33.3930015564</v>
+        <v>18.4297008514</v>
       </c>
       <c r="D204" t="n">
-        <v>-70.7857971191</v>
+        <v>-69.6688995361</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>Santo Domingo</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>SDQ</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Santo Domingo, Dominican Republic</t>
+          <t>São José do Rio Preto, Brazil</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>18.4297008514</v>
+        <v>-20.807157</v>
       </c>
       <c r="D205" t="n">
-        <v>-69.6688995361</v>
+        <v>-49.378994</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>DO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>Santo Domingo</t>
+          <t>São José do Rio Preto</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SJK</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>São José do Rio Preto, Brazil</t>
+          <t>São José dos Campos, Brazil</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>-20.807157</v>
+        <v>-23.1791</v>
       </c>
       <c r="D206" t="n">
-        <v>-49.378994</v>
+        <v>-45.8872</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -6847,26 +6847,26 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>São José dos Campos</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>SJK</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>São José dos Campos, Brazil</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>-23.1791</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="D207" t="n">
-        <v>-45.8872</v>
+        <v>-46.4730567932</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -6880,26 +6880,26 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>São José dos Campos</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>-23.4355564117</v>
+        <v>-23.54389</v>
       </c>
       <c r="D208" t="n">
-        <v>-46.4730567932</v>
+        <v>-46.63445</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -6913,30 +6913,30 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Sorocaba</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>-23.54389</v>
+        <v>12.007116</v>
       </c>
       <c r="D209" t="n">
-        <v>-46.63445</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -6946,30 +6946,30 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>12.007116</v>
+        <v>14.0608</v>
       </c>
       <c r="D210" t="n">
-        <v>-61.7882288</v>
+        <v>-87.21720000000001</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -6979,30 +6979,30 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>NVT</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>Timbó, Brazil</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>14.0608</v>
+        <v>-26.8251</v>
       </c>
       <c r="D211" t="n">
-        <v>-87.21720000000001</v>
+        <v>-49.2695</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -7012,26 +7012,26 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>Timbo</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>NVT</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Timbó, Brazil</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>-26.8251</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="D212" t="n">
-        <v>-49.2695</v>
+        <v>-48.225276947</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -7045,26 +7045,26 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>Timbo</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>VIX</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Vitoria, Brazil</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>-18.8836116791</v>
+        <v>-20.64871</v>
       </c>
       <c r="D213" t="n">
-        <v>-48.225276947</v>
+        <v>-41.90857</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -7078,30 +7078,30 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Vitoria</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>VIX</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Vitoria, Brazil</t>
+          <t>Willemstad, Curaçao</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>-20.64871</v>
+        <v>12.1888999939</v>
       </c>
       <c r="D214" t="n">
-        <v>-41.90857</v>
+        <v>-68.95980072019999</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -7111,30 +7111,30 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Willemstad</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>CAW</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Campos dos Goytacazes, Brazil</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>12.1888999939</v>
+        <v>-21.698299408</v>
       </c>
       <c r="D215" t="n">
-        <v>-68.95980072019999</v>
+        <v>-41.301700592</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -7144,63 +7144,63 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Campos dos Goytacazes</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>CAW</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes, Brazil</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>-21.698299408</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D216" t="n">
-        <v>-41.301700592</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>31.7226009369</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D217" t="n">
-        <v>35.9931983948</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7210,30 +7210,30 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>38.7463989258</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D218" t="n">
-        <v>48.8180007935</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -7243,30 +7243,30 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>33.2625007629</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D219" t="n">
-        <v>44.2346000671</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7276,30 +7276,30 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>40.4674987793</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D220" t="n">
-        <v>50.0466995239</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7309,30 +7309,30 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>30.5491008759</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D221" t="n">
-        <v>47.6621017456</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -7342,30 +7342,30 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>33.8208999634</v>
+        <v>26.471200943</v>
       </c>
       <c r="D222" t="n">
-        <v>35.4883995056</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7375,30 +7375,30 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>26.471200943</v>
+        <v>25.2605946</v>
       </c>
       <c r="D223" t="n">
-        <v>49.7979011536</v>
+        <v>51.6137665</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7408,30 +7408,30 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>25.2605946</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D224" t="n">
-        <v>51.6137665</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7441,30 +7441,30 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>25.2527999878</v>
+        <v>36.1901</v>
       </c>
       <c r="D225" t="n">
-        <v>55.3643989563</v>
+        <v>43.993</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -7474,30 +7474,30 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>36.1901</v>
+        <v>32.78492</v>
       </c>
       <c r="D226" t="n">
-        <v>43.993</v>
+        <v>34.96069</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -7507,30 +7507,30 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>32.78492</v>
+        <v>21.679599762</v>
       </c>
       <c r="D227" t="n">
-        <v>34.96069</v>
+        <v>39.15650177</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -7540,30 +7540,30 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>21.679599762</v>
+        <v>29.226600647</v>
       </c>
       <c r="D228" t="n">
-        <v>39.15650177</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -7573,30 +7573,30 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>29.226600647</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D229" t="n">
-        <v>47.9688987732</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7606,30 +7606,30 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>26.2707996368</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D230" t="n">
-        <v>50.6335983276</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -7639,30 +7639,30 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>23.5932998657</v>
+        <v>31.989722</v>
       </c>
       <c r="D231" t="n">
-        <v>58.2844009399</v>
+        <v>44.404167</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -7672,26 +7672,26 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>31.989722</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D232" t="n">
-        <v>44.404167</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -7705,30 +7705,30 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>30.9358005524</v>
+        <v>32.2719</v>
       </c>
       <c r="D233" t="n">
-        <v>46.0900993347</v>
+        <v>35.0194</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -7738,30 +7738,30 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>32.2719</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D234" t="n">
-        <v>35.0194</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -7771,30 +7771,30 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>24.9575996399</v>
+        <v>35.5668</v>
       </c>
       <c r="D235" t="n">
-        <v>46.6987991333</v>
+        <v>45.4161</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -7804,30 +7804,30 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>35.5668</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D236" t="n">
-        <v>45.4161</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -7837,59 +7837,59 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>32.0113983154</v>
+        <v>38.94449997</v>
       </c>
       <c r="D237" t="n">
-        <v>34.8866996765</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>38.94449997</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D238" t="n">
-        <v>-77.45580292</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -7903,26 +7903,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>33.6366996765</v>
+        <v>42.36429977</v>
       </c>
       <c r="D239" t="n">
-        <v>-84.4281005859</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7936,26 +7936,26 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>42.36429977</v>
+        <v>42.94049835</v>
       </c>
       <c r="D240" t="n">
-        <v>-71.00520324999999</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -7969,30 +7969,30 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>42.94049835</v>
+        <v>51.113899231</v>
       </c>
       <c r="D241" t="n">
-        <v>-78.73220062</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -8002,30 +8002,30 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>51.113899231</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D242" t="n">
-        <v>-114.019996643</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -8035,26 +8035,26 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>35.2140007019</v>
+        <v>41.97859955</v>
       </c>
       <c r="D243" t="n">
-        <v>-80.94309997560001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -8068,26 +8068,26 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>41.97859955</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D244" t="n">
-        <v>-87.90480042</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -8101,26 +8101,26 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>39.9980010986</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D245" t="n">
-        <v>-82.89189910890001</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -8134,26 +8134,26 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>32.8968009949</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D246" t="n">
-        <v>-97.0380020142</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -8167,26 +8167,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>39.8616981506</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D247" t="n">
-        <v>-104.672996521</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8200,26 +8200,26 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>42.2123985291</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D248" t="n">
-        <v>-83.35340118409999</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8233,26 +8233,26 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>21.3187007904</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D249" t="n">
-        <v>-157.9219970703</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8266,26 +8266,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>29.9843997955</v>
+        <v>39.717300415</v>
       </c>
       <c r="D250" t="n">
-        <v>-95.34140014650001</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8299,26 +8299,26 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>39.717300415</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D251" t="n">
-        <v>-86.2944030762</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8332,26 +8332,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>30.4941005707</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D252" t="n">
-        <v>-81.68789672849999</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8365,26 +8365,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>39.2975997925</v>
+        <v>36.08010101</v>
       </c>
       <c r="D253" t="n">
-        <v>-94.7138977051</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8398,26 +8398,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>36.08010101</v>
+        <v>33.94250107</v>
       </c>
       <c r="D254" t="n">
-        <v>-115.1520004</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8431,26 +8431,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>33.94250107</v>
+        <v>26.17580032</v>
       </c>
       <c r="D255" t="n">
-        <v>-118.4079971</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8464,26 +8464,26 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>26.17580032</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D256" t="n">
-        <v>-98.23860168</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -8497,30 +8497,30 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>35.0424003601</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D257" t="n">
-        <v>-89.9766998291</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -8530,30 +8530,30 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>19.4363002777</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D258" t="n">
-        <v>-99.07209777830001</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -8563,26 +8563,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>25.7931995392</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D259" t="n">
-        <v>-80.2906036377</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8596,26 +8596,26 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>44.8819999695</v>
+        <v>32.30059814</v>
       </c>
       <c r="D260" t="n">
-        <v>-93.22180175779999</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -8629,30 +8629,30 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>32.30059814</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D261" t="n">
-        <v>-86.39399718999999</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -8662,30 +8662,30 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>45.4706001282</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D262" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -8695,26 +8695,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>36.1245002747</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D263" t="n">
-        <v>-86.6781997681</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8728,26 +8728,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>40.6925010681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D264" t="n">
-        <v>-74.1687011719</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8761,26 +8761,26 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>36.8945999146</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D265" t="n">
-        <v>-76.2012023926</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -8794,30 +8794,30 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>41.3031997681</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D266" t="n">
-        <v>-95.89409637449999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -8827,30 +8827,30 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>45.3224983215</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D267" t="n">
-        <v>-75.66919708250001</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -8860,26 +8860,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>39.8718986511</v>
+        <v>33.434299469</v>
       </c>
       <c r="D268" t="n">
-        <v>-75.24109649659999</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8893,26 +8893,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>33.434299469</v>
+        <v>40.49150085</v>
       </c>
       <c r="D269" t="n">
-        <v>-112.012001038</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8926,26 +8926,26 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>40.49150085</v>
+        <v>45.58869934</v>
       </c>
       <c r="D270" t="n">
-        <v>-80.23290253</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -8959,30 +8959,30 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>45.58869934</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D271" t="n">
-        <v>-122.5979996</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -8992,30 +8992,30 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>20.6173000336</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D272" t="n">
-        <v>-100.185997009</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -9025,26 +9025,26 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>37.5051994324</v>
+        <v>38.695400238</v>
       </c>
       <c r="D273" t="n">
-        <v>-77.3197021484</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -9058,26 +9058,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>38.695400238</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D274" t="n">
-        <v>-121.591003418</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -9091,26 +9091,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>40.7883987427</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D275" t="n">
-        <v>-111.977996826</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9124,26 +9124,26 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>32.7336006165</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D276" t="n">
-        <v>-117.190002441</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -9157,30 +9157,30 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>37.3625984192</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D277" t="n">
-        <v>-121.929000855</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9190,30 +9190,30 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>52.1707992554</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D278" t="n">
-        <v>-106.699996948</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -9223,26 +9223,26 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>47.4490013123</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D279" t="n">
-        <v>-122.308998108</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -9256,26 +9256,26 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>43.540819819502</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D280" t="n">
-        <v>-96.65511577730963</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -9289,26 +9289,26 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>38.7486991882</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D281" t="n">
-        <v>-90.37000274659999</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -9322,30 +9322,30 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>30.3964996338</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D282" t="n">
-        <v>-84.3503036499</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -9355,26 +9355,26 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>43.6772003174</v>
+        <v>49.193901062</v>
       </c>
       <c r="D283" t="n">
-        <v>-79.63059997560001</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -9388,26 +9388,26 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>49.193901062</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D284" t="n">
-        <v>-123.183998108</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -9421,30 +9421,30 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>49.9099998474</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D285" t="n">
-        <v>-97.2398986816</v>
+        <v>-122.375</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -9454,30 +9454,30 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>37.6189994812</v>
+        <v>17.9951</v>
       </c>
       <c r="D286" t="n">
-        <v>-122.375</v>
+        <v>-76.7846</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9487,30 +9487,30 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>17.9951</v>
+        <v>44.8081</v>
       </c>
       <c r="D287" t="n">
-        <v>-76.7846</v>
+        <v>-68.795</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -9520,26 +9520,26 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>44.8081</v>
+        <v>30.1975</v>
       </c>
       <c r="D288" t="n">
-        <v>-68.795</v>
+        <v>-97.6664</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -9553,26 +9553,26 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>30.1975</v>
+        <v>35.0844</v>
       </c>
       <c r="D289" t="n">
-        <v>-97.6664</v>
+        <v>-106.6504</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -9586,30 +9586,30 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>35.0844</v>
+        <v>20.5217990875</v>
       </c>
       <c r="D290" t="n">
-        <v>-106.6504</v>
+        <v>-103.3109970093</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -9619,63 +9619,63 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Guadalajara</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>20.5217990875</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D291" t="n">
-        <v>-103.3109970093</v>
+        <v>138.5335637</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>-34.9431729</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D292" t="n">
-        <v>138.5335637</v>
+        <v>174.792007446</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -9685,30 +9685,30 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>-37.0080986023</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D293" t="n">
-        <v>174.792007446</v>
+        <v>153.117004394</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -9718,26 +9718,26 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>-27.3841991425</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D294" t="n">
-        <v>153.117004394</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -9751,30 +9751,30 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>-35.3069000244</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D295" t="n">
-        <v>149.1950073242</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
@@ -9784,92 +9784,92 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>-43.4893989563</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D296" t="n">
-        <v>172.5319976807</v>
+        <v>144.796005249</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>13.4834003448</v>
+        <v>-42.883209</v>
       </c>
       <c r="D297" t="n">
-        <v>144.796005249</v>
+        <v>147.331665</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>-42.883209</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D298" t="n">
-        <v>147.331665</v>
+        <v>144.843002319</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -9883,30 +9883,30 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>-37.6733016968</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D299" t="n">
-        <v>144.843002319</v>
+        <v>166.212997436</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -9916,30 +9916,30 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>-22.0146007538</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D300" t="n">
-        <v>166.212997436</v>
+        <v>115.967002869</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -9949,26 +9949,26 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>-31.9402999878</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D301" t="n">
-        <v>115.967002869</v>
+        <v>151.177001953</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -9982,30 +9982,30 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PPT</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Tahiti, French Polynesia</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>-33.9460983276</v>
+        <v>-17.5536994934</v>
       </c>
       <c r="D302" t="n">
-        <v>151.177001953</v>
+        <v>-149.606994629</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -10014,39 +10014,6 @@
         </is>
       </c>
       <c r="G302" t="inlineStr">
-        <is>
-          <t>Sydney</t>
-        </is>
-      </c>
-    </row>
-    <row r="303">
-      <c r="A303" s="1" t="inlineStr">
-        <is>
-          <t>PPT</t>
-        </is>
-      </c>
-      <c r="B303" t="inlineStr">
-        <is>
-          <t>Tahiti, French Polynesia</t>
-        </is>
-      </c>
-      <c r="C303" t="n">
-        <v>-17.5536994934</v>
-      </c>
-      <c r="D303" t="n">
-        <v>-149.606994629</v>
-      </c>
-      <c r="E303" t="inlineStr">
-        <is>
-          <t>PF</t>
-        </is>
-      </c>
-      <c r="F303" t="inlineStr">
-        <is>
-          <t>Oceania</t>
-        </is>
-      </c>
-      <c r="G303" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 8ccd22bd7e9cde14ad1e32f411e4e2738a2f1523
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G302"/>
+  <dimension ref="A1:G301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5864,23 +5864,23 @@
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>CCP</t>
+          <t>COR</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Concepción, Chile</t>
+          <t>Córdoba, Argentina</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>-36.8201</v>
+        <v>-31.31</v>
       </c>
       <c r="D177" t="n">
-        <v>-73.0444</v>
+        <v>-64.208333</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -5890,30 +5890,30 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>Concepción</t>
+          <t>Córdoba</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>COR</t>
+          <t>CGB</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Córdoba, Argentina</t>
+          <t>Cuiabá, Brazil</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>-31.31</v>
+        <v>-15.59611</v>
       </c>
       <c r="D178" t="n">
-        <v>-64.208333</v>
+        <v>-56.09667</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -5923,26 +5923,26 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Cuiaba</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>CGB</t>
+          <t>CWB</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Cuiabá, Brazil</t>
+          <t>Curitiba, Brazil</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>-15.59611</v>
+        <v>-25.5284996033</v>
       </c>
       <c r="D179" t="n">
-        <v>-56.09667</v>
+        <v>-49.1758003235</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -5956,26 +5956,26 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>Cuiaba</t>
+          <t>Curitiba</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>CWB</t>
+          <t>FLN</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Curitiba, Brazil</t>
+          <t>Florianopolis, Brazil</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>-25.5284996033</v>
+        <v>-27.6702785492</v>
       </c>
       <c r="D180" t="n">
-        <v>-49.1758003235</v>
+        <v>-48.5525016785</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -5989,26 +5989,26 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>Curitiba</t>
+          <t>Florianopolis</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>FLN</t>
+          <t>FOR</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Florianopolis, Brazil</t>
+          <t>Fortaleza, Brazil</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>-27.6702785492</v>
+        <v>-3.7762799263</v>
       </c>
       <c r="D181" t="n">
-        <v>-48.5525016785</v>
+        <v>-38.5326004028</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -6022,30 +6022,30 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>Florianopolis</t>
+          <t>Fortaleza</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>FOR</t>
+          <t>GEO</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Fortaleza, Brazil</t>
+          <t>Georgetown, Guyana</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>-3.7762799263</v>
+        <v>6.825648</v>
       </c>
       <c r="D182" t="n">
-        <v>-38.5326004028</v>
+        <v>-58.163756</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GY</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -6055,30 +6055,30 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Georgetown</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>GEO</t>
+          <t>GYN</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Georgetown, Guyana</t>
+          <t>Goiânia, Brazil</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>6.825648</v>
+        <v>-16.69727</v>
       </c>
       <c r="D183" t="n">
-        <v>-58.163756</v>
+        <v>-49.26851</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>GY</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -6088,96 +6088,96 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>Georgetown</t>
+          <t>Goiania</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>GYN</t>
+          <t>GUA</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Goiânia, Brazil</t>
+          <t>Guatemala City, Guatemala</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>-16.69727</v>
+        <v>14.5832996368</v>
       </c>
       <c r="D184" t="n">
-        <v>-49.26851</v>
+        <v>-90.5274963379</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GT</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>Goiania</t>
+          <t>Guatemala City</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>GUA</t>
+          <t>GYE</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Guatemala City, Guatemala</t>
+          <t>Guayaquil, Ecuador</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>14.5832996368</v>
+        <v>-2.1894</v>
       </c>
       <c r="D185" t="n">
-        <v>-90.5274963379</v>
+        <v>-79.8891</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>GT</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>Guatemala City</t>
+          <t>Guayaquil</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>GYE</t>
+          <t>ITJ</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Guayaquil, Ecuador</t>
+          <t>Itajaí, Brazil</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>-2.1894</v>
+        <v>-27.6116676331</v>
       </c>
       <c r="D186" t="n">
-        <v>-79.8891</v>
+        <v>-48.6727790833</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -6187,26 +6187,26 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>Guayaquil</t>
+          <t>Itajai</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
         <is>
-          <t>ITJ</t>
+          <t>JOI</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Itajaí, Brazil</t>
+          <t>Joinville, Brazil</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>-27.6116676331</v>
+        <v>-26.304408</v>
       </c>
       <c r="D187" t="n">
-        <v>-48.6727790833</v>
+        <v>-48.846383</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -6220,26 +6220,26 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>Itajai</t>
+          <t>Joinville</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
         <is>
-          <t>JOI</t>
+          <t>JDO</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Joinville, Brazil</t>
+          <t>Juazeiro do Norte, Brazil</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>-26.304408</v>
+        <v>-7.2242</v>
       </c>
       <c r="D188" t="n">
-        <v>-48.846383</v>
+        <v>-39.313</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -6253,30 +6253,30 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>Joinville</t>
+          <t>Juazeiro do Norte</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>JDO</t>
+          <t>LIM</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte, Brazil</t>
+          <t>Lima, Peru</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>-7.2242</v>
+        <v>-12.021900177</v>
       </c>
       <c r="D189" t="n">
-        <v>-39.313</v>
+        <v>-77.1143035889</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -6286,30 +6286,30 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte</t>
+          <t>Lima</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
         <is>
-          <t>LIM</t>
+          <t>MAO</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Lima, Peru</t>
+          <t>Manaus, Brazil</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>-12.021900177</v>
+        <v>-3.11286</v>
       </c>
       <c r="D190" t="n">
-        <v>-77.1143035889</v>
+        <v>-60.01949</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -6319,30 +6319,30 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>Lima</t>
+          <t>Manaus</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
         <is>
-          <t>MAO</t>
+          <t>MDE</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Manaus, Brazil</t>
+          <t>Medellín, Colombia</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>-3.11286</v>
+        <v>6.16454</v>
       </c>
       <c r="D191" t="n">
-        <v>-60.01949</v>
+        <v>-75.42310000000001</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -6352,30 +6352,30 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>Manaus</t>
+          <t>Medellín</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
         <is>
-          <t>MDE</t>
+          <t>NQN</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Medellín, Colombia</t>
+          <t>Neuquén, Argentina</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>6.16454</v>
+        <v>-38.9490013123</v>
       </c>
       <c r="D192" t="n">
-        <v>-75.42310000000001</v>
+        <v>-68.1557006836</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -6385,30 +6385,30 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>Medellín</t>
+          <t>Neuquen</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
         <is>
-          <t>NQN</t>
+          <t>PTY</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Neuquén, Argentina</t>
+          <t>Panama City, Panama</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>-38.9490013123</v>
+        <v>9.0713596344</v>
       </c>
       <c r="D193" t="n">
-        <v>-68.1557006836</v>
+        <v>-79.3834991455</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -6418,30 +6418,30 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>Neuquen</t>
+          <t>Panama City</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
         <is>
-          <t>PTY</t>
+          <t>PBM</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Panama City, Panama</t>
+          <t>Paramaribo, Suriname</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>9.0713596344</v>
+        <v>5.452831</v>
       </c>
       <c r="D194" t="n">
-        <v>-79.3834991455</v>
+        <v>-55.187783</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>SR</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -6451,30 +6451,30 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>Panama City</t>
+          <t>Paramaribo</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
         <is>
-          <t>PBM</t>
+          <t>POA</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Paramaribo, Suriname</t>
+          <t>Porto Alegre, Brazil</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>5.452831</v>
+        <v>-29.9944000244</v>
       </c>
       <c r="D195" t="n">
-        <v>-55.187783</v>
+        <v>-51.1713981628</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>SR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -6484,30 +6484,30 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>Paramaribo</t>
+          <t>Porto Alegre</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
         <is>
-          <t>POA</t>
+          <t>UIO</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Porto Alegre, Brazil</t>
+          <t>Quito, Ecuador</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>-29.9944000244</v>
+        <v>-0.1291666667</v>
       </c>
       <c r="D196" t="n">
-        <v>-51.1713981628</v>
+        <v>-78.3575</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -6517,30 +6517,30 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>Porto Alegre</t>
+          <t>Quito</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>UIO</t>
+          <t>REC</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Quito, Ecuador</t>
+          <t>Recife, Brazil</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>-0.1291666667</v>
+        <v>-8.126489639300001</v>
       </c>
       <c r="D197" t="n">
-        <v>-78.3575</v>
+        <v>-34.9235992432</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -6550,26 +6550,26 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Quito</t>
+          <t>Recife</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Recife, Brazil</t>
+          <t>Ribeirao Preto, Brazil</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>-8.126489639300001</v>
+        <v>-21.1363887787</v>
       </c>
       <c r="D198" t="n">
-        <v>-34.9235992432</v>
+        <v>-47.7766685486</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -6583,26 +6583,26 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>Ribeirao Preto</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>GIG</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Ribeirao Preto, Brazil</t>
+          <t>Rio de Janeiro, Brazil</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>-21.1363887787</v>
+        <v>-22.8099994659</v>
       </c>
       <c r="D199" t="n">
-        <v>-47.7766685486</v>
+        <v>-43.2505569458</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -6616,26 +6616,26 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>Ribeirao Preto</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>GIG</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Rio de Janeiro, Brazil</t>
+          <t>Salvador, Brazil</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>-22.8099994659</v>
+        <v>-12.9086112976</v>
       </c>
       <c r="D200" t="n">
-        <v>-43.2505569458</v>
+        <v>-38.3224983215</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -6649,30 +6649,30 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Salvador, Brazil</t>
+          <t>San José, Costa Rica</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>-12.9086112976</v>
+        <v>9.9938602448</v>
       </c>
       <c r="D201" t="n">
-        <v>-38.3224983215</v>
+        <v>-84.2088012695</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -6682,30 +6682,30 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>Salvador</t>
+          <t>San José</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>San José, Costa Rica</t>
+          <t>Santiago, Chile</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>9.9938602448</v>
+        <v>-33.3930015564</v>
       </c>
       <c r="D202" t="n">
-        <v>-84.2088012695</v>
+        <v>-70.7857971191</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -6715,92 +6715,92 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Santiago</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SDQ</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Santiago, Chile</t>
+          <t>Santo Domingo, Dominican Republic</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>-33.3930015564</v>
+        <v>18.4297008514</v>
       </c>
       <c r="D203" t="n">
-        <v>-70.7857971191</v>
+        <v>-69.6688995361</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>Santo Domingo</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>SDQ</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Santo Domingo, Dominican Republic</t>
+          <t>São José do Rio Preto, Brazil</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>18.4297008514</v>
+        <v>-20.807157</v>
       </c>
       <c r="D204" t="n">
-        <v>-69.6688995361</v>
+        <v>-49.378994</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>DO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>Santo Domingo</t>
+          <t>São José do Rio Preto</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SJK</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>São José do Rio Preto, Brazil</t>
+          <t>São José dos Campos, Brazil</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>-20.807157</v>
+        <v>-23.1791</v>
       </c>
       <c r="D205" t="n">
-        <v>-49.378994</v>
+        <v>-45.8872</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -6814,26 +6814,26 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>São José dos Campos</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>SJK</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>São José dos Campos, Brazil</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>-23.1791</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="D206" t="n">
-        <v>-45.8872</v>
+        <v>-46.4730567932</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -6847,26 +6847,26 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>São José dos Campos</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>-23.4355564117</v>
+        <v>-23.54389</v>
       </c>
       <c r="D207" t="n">
-        <v>-46.4730567932</v>
+        <v>-46.63445</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -6880,30 +6880,30 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Sorocaba</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>-23.54389</v>
+        <v>12.007116</v>
       </c>
       <c r="D208" t="n">
-        <v>-46.63445</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -6913,30 +6913,30 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>12.007116</v>
+        <v>14.0608</v>
       </c>
       <c r="D209" t="n">
-        <v>-61.7882288</v>
+        <v>-87.21720000000001</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -6946,30 +6946,30 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>NVT</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>Timbó, Brazil</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>14.0608</v>
+        <v>-26.8251</v>
       </c>
       <c r="D210" t="n">
-        <v>-87.21720000000001</v>
+        <v>-49.2695</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -6979,26 +6979,26 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>Timbo</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>NVT</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Timbó, Brazil</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>-26.8251</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="D211" t="n">
-        <v>-49.2695</v>
+        <v>-48.225276947</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -7012,26 +7012,26 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>Timbo</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>VIX</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Vitoria, Brazil</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>-18.8836116791</v>
+        <v>-20.64871</v>
       </c>
       <c r="D212" t="n">
-        <v>-48.225276947</v>
+        <v>-41.90857</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -7045,30 +7045,30 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Vitoria</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>VIX</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Vitoria, Brazil</t>
+          <t>Willemstad, Curaçao</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>-20.64871</v>
+        <v>12.1888999939</v>
       </c>
       <c r="D213" t="n">
-        <v>-41.90857</v>
+        <v>-68.95980072019999</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -7078,30 +7078,30 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Willemstad</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>CAW</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Campos dos Goytacazes, Brazil</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>12.1888999939</v>
+        <v>-21.698299408</v>
       </c>
       <c r="D214" t="n">
-        <v>-68.95980072019999</v>
+        <v>-41.301700592</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -7111,63 +7111,63 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Campos dos Goytacazes</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>CAW</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes, Brazil</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>-21.698299408</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D215" t="n">
-        <v>-41.301700592</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>31.7226009369</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D216" t="n">
-        <v>35.9931983948</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -7177,30 +7177,30 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>38.7463989258</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D217" t="n">
-        <v>48.8180007935</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7210,30 +7210,30 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>33.2625007629</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D218" t="n">
-        <v>44.2346000671</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -7243,30 +7243,30 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>40.4674987793</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D219" t="n">
-        <v>50.0466995239</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7276,30 +7276,30 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>30.5491008759</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D220" t="n">
-        <v>47.6621017456</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7309,30 +7309,30 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>33.8208999634</v>
+        <v>26.471200943</v>
       </c>
       <c r="D221" t="n">
-        <v>35.4883995056</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -7342,30 +7342,30 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>26.471200943</v>
+        <v>25.2605946</v>
       </c>
       <c r="D222" t="n">
-        <v>49.7979011536</v>
+        <v>51.6137665</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7375,30 +7375,30 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>25.2605946</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D223" t="n">
-        <v>51.6137665</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7408,30 +7408,30 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>25.2527999878</v>
+        <v>36.1901</v>
       </c>
       <c r="D224" t="n">
-        <v>55.3643989563</v>
+        <v>43.993</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7441,30 +7441,30 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>36.1901</v>
+        <v>32.78492</v>
       </c>
       <c r="D225" t="n">
-        <v>43.993</v>
+        <v>34.96069</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -7474,30 +7474,30 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>32.78492</v>
+        <v>21.679599762</v>
       </c>
       <c r="D226" t="n">
-        <v>34.96069</v>
+        <v>39.15650177</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -7507,30 +7507,30 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>21.679599762</v>
+        <v>29.226600647</v>
       </c>
       <c r="D227" t="n">
-        <v>39.15650177</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -7540,30 +7540,30 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>29.226600647</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D228" t="n">
-        <v>47.9688987732</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -7573,30 +7573,30 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>26.2707996368</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D229" t="n">
-        <v>50.6335983276</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7606,30 +7606,30 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>23.5932998657</v>
+        <v>31.989722</v>
       </c>
       <c r="D230" t="n">
-        <v>58.2844009399</v>
+        <v>44.404167</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -7639,26 +7639,26 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>31.989722</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D231" t="n">
-        <v>44.404167</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -7672,30 +7672,30 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>30.9358005524</v>
+        <v>32.2719</v>
       </c>
       <c r="D232" t="n">
-        <v>46.0900993347</v>
+        <v>35.0194</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -7705,30 +7705,30 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>32.2719</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D233" t="n">
-        <v>35.0194</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -7738,30 +7738,30 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>24.9575996399</v>
+        <v>35.5668</v>
       </c>
       <c r="D234" t="n">
-        <v>46.6987991333</v>
+        <v>45.4161</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -7771,30 +7771,30 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>35.5668</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D235" t="n">
-        <v>45.4161</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -7804,59 +7804,59 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>32.0113983154</v>
+        <v>38.94449997</v>
       </c>
       <c r="D236" t="n">
-        <v>34.8866996765</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>38.94449997</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D237" t="n">
-        <v>-77.45580292</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -7870,26 +7870,26 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>33.6366996765</v>
+        <v>42.36429977</v>
       </c>
       <c r="D238" t="n">
-        <v>-84.4281005859</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -7903,26 +7903,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>42.36429977</v>
+        <v>42.94049835</v>
       </c>
       <c r="D239" t="n">
-        <v>-71.00520324999999</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7936,30 +7936,30 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>42.94049835</v>
+        <v>51.113899231</v>
       </c>
       <c r="D240" t="n">
-        <v>-78.73220062</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -7969,30 +7969,30 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>51.113899231</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D241" t="n">
-        <v>-114.019996643</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -8002,26 +8002,26 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>35.2140007019</v>
+        <v>41.97859955</v>
       </c>
       <c r="D242" t="n">
-        <v>-80.94309997560001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -8035,26 +8035,26 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>41.97859955</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D243" t="n">
-        <v>-87.90480042</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -8068,26 +8068,26 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>39.9980010986</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D244" t="n">
-        <v>-82.89189910890001</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -8101,26 +8101,26 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>32.8968009949</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D245" t="n">
-        <v>-97.0380020142</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -8134,26 +8134,26 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>39.8616981506</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D246" t="n">
-        <v>-104.672996521</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -8167,26 +8167,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>42.2123985291</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D247" t="n">
-        <v>-83.35340118409999</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8200,26 +8200,26 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>21.3187007904</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D248" t="n">
-        <v>-157.9219970703</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8233,26 +8233,26 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>29.9843997955</v>
+        <v>39.717300415</v>
       </c>
       <c r="D249" t="n">
-        <v>-95.34140014650001</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8266,26 +8266,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>39.717300415</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D250" t="n">
-        <v>-86.2944030762</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8299,26 +8299,26 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>30.4941005707</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D251" t="n">
-        <v>-81.68789672849999</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8332,26 +8332,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>39.2975997925</v>
+        <v>36.08010101</v>
       </c>
       <c r="D252" t="n">
-        <v>-94.7138977051</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8365,26 +8365,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>36.08010101</v>
+        <v>33.94250107</v>
       </c>
       <c r="D253" t="n">
-        <v>-115.1520004</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8398,26 +8398,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>33.94250107</v>
+        <v>26.17580032</v>
       </c>
       <c r="D254" t="n">
-        <v>-118.4079971</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8431,26 +8431,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>26.17580032</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D255" t="n">
-        <v>-98.23860168</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8464,30 +8464,30 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>35.0424003601</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D256" t="n">
-        <v>-89.9766998291</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -8497,30 +8497,30 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>19.4363002777</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D257" t="n">
-        <v>-99.07209777830001</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -8530,26 +8530,26 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>25.7931995392</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D258" t="n">
-        <v>-80.2906036377</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8563,26 +8563,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>44.8819999695</v>
+        <v>32.30059814</v>
       </c>
       <c r="D259" t="n">
-        <v>-93.22180175779999</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8596,30 +8596,30 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>32.30059814</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D260" t="n">
-        <v>-86.39399718999999</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -8629,30 +8629,30 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>45.4706001282</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D261" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -8662,26 +8662,26 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>36.1245002747</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D262" t="n">
-        <v>-86.6781997681</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8695,26 +8695,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>40.6925010681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D263" t="n">
-        <v>-74.1687011719</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8728,26 +8728,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>36.8945999146</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D264" t="n">
-        <v>-76.2012023926</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8761,30 +8761,30 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>41.3031997681</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D265" t="n">
-        <v>-95.89409637449999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -8794,30 +8794,30 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>45.3224983215</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D266" t="n">
-        <v>-75.66919708250001</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -8827,26 +8827,26 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>39.8718986511</v>
+        <v>33.434299469</v>
       </c>
       <c r="D267" t="n">
-        <v>-75.24109649659999</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -8860,26 +8860,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>33.434299469</v>
+        <v>40.49150085</v>
       </c>
       <c r="D268" t="n">
-        <v>-112.012001038</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8893,26 +8893,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>40.49150085</v>
+        <v>45.58869934</v>
       </c>
       <c r="D269" t="n">
-        <v>-80.23290253</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8926,30 +8926,30 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>45.58869934</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D270" t="n">
-        <v>-122.5979996</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -8959,30 +8959,30 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>20.6173000336</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D271" t="n">
-        <v>-100.185997009</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -8992,26 +8992,26 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>37.5051994324</v>
+        <v>38.695400238</v>
       </c>
       <c r="D272" t="n">
-        <v>-77.3197021484</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -9025,26 +9025,26 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>38.695400238</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D273" t="n">
-        <v>-121.591003418</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -9058,26 +9058,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>40.7883987427</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D274" t="n">
-        <v>-111.977996826</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -9091,26 +9091,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>32.7336006165</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D275" t="n">
-        <v>-117.190002441</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9124,30 +9124,30 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>37.3625984192</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D276" t="n">
-        <v>-121.929000855</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -9157,30 +9157,30 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>52.1707992554</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D277" t="n">
-        <v>-106.699996948</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9190,26 +9190,26 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>47.4490013123</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D278" t="n">
-        <v>-122.308998108</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -9223,26 +9223,26 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>43.540819819502</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D279" t="n">
-        <v>-96.65511577730963</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -9256,26 +9256,26 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>38.7486991882</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D280" t="n">
-        <v>-90.37000274659999</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -9289,30 +9289,30 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>30.3964996338</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D281" t="n">
-        <v>-84.3503036499</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -9322,26 +9322,26 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>43.6772003174</v>
+        <v>49.193901062</v>
       </c>
       <c r="D282" t="n">
-        <v>-79.63059997560001</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -9355,26 +9355,26 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>49.193901062</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D283" t="n">
-        <v>-123.183998108</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -9388,30 +9388,30 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>49.9099998474</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D284" t="n">
-        <v>-97.2398986816</v>
+        <v>-122.375</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -9421,30 +9421,30 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>37.6189994812</v>
+        <v>17.9951</v>
       </c>
       <c r="D285" t="n">
-        <v>-122.375</v>
+        <v>-76.7846</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -9454,30 +9454,30 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>17.9951</v>
+        <v>44.8081</v>
       </c>
       <c r="D286" t="n">
-        <v>-76.7846</v>
+        <v>-68.795</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9487,26 +9487,26 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>44.8081</v>
+        <v>30.1975</v>
       </c>
       <c r="D287" t="n">
-        <v>-68.795</v>
+        <v>-97.6664</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -9520,26 +9520,26 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>30.1975</v>
+        <v>35.0844</v>
       </c>
       <c r="D288" t="n">
-        <v>-97.6664</v>
+        <v>-106.6504</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -9553,30 +9553,30 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>35.0844</v>
+        <v>20.5217990875</v>
       </c>
       <c r="D289" t="n">
-        <v>-106.6504</v>
+        <v>-103.3109970093</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -9586,63 +9586,63 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Guadalajara</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>20.5217990875</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D290" t="n">
-        <v>-103.3109970093</v>
+        <v>138.5335637</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>-34.9431729</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D291" t="n">
-        <v>138.5335637</v>
+        <v>174.792007446</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -9652,30 +9652,30 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>-37.0080986023</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D292" t="n">
-        <v>174.792007446</v>
+        <v>153.117004394</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -9685,26 +9685,26 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>-27.3841991425</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D293" t="n">
-        <v>153.117004394</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -9718,30 +9718,30 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>-35.3069000244</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D294" t="n">
-        <v>149.1950073242</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -9751,92 +9751,92 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>-43.4893989563</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D295" t="n">
-        <v>172.5319976807</v>
+        <v>144.796005249</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>13.4834003448</v>
+        <v>-42.883209</v>
       </c>
       <c r="D296" t="n">
-        <v>144.796005249</v>
+        <v>147.331665</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>-42.883209</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D297" t="n">
-        <v>147.331665</v>
+        <v>144.843002319</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -9850,30 +9850,30 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>-37.6733016968</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D298" t="n">
-        <v>144.843002319</v>
+        <v>166.212997436</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -9883,30 +9883,30 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>-22.0146007538</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D299" t="n">
-        <v>166.212997436</v>
+        <v>115.967002869</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -9916,26 +9916,26 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>-31.9402999878</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D300" t="n">
-        <v>115.967002869</v>
+        <v>151.177001953</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -9949,30 +9949,30 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PPT</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Tahiti, French Polynesia</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>-33.9460983276</v>
+        <v>-17.5536994934</v>
       </c>
       <c r="D301" t="n">
-        <v>151.177001953</v>
+        <v>-149.606994629</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -9981,39 +9981,6 @@
         </is>
       </c>
       <c r="G301" t="inlineStr">
-        <is>
-          <t>Sydney</t>
-        </is>
-      </c>
-    </row>
-    <row r="302">
-      <c r="A302" s="1" t="inlineStr">
-        <is>
-          <t>PPT</t>
-        </is>
-      </c>
-      <c r="B302" t="inlineStr">
-        <is>
-          <t>Tahiti, French Polynesia</t>
-        </is>
-      </c>
-      <c r="C302" t="n">
-        <v>-17.5536994934</v>
-      </c>
-      <c r="D302" t="n">
-        <v>-149.606994629</v>
-      </c>
-      <c r="E302" t="inlineStr">
-        <is>
-          <t>PF</t>
-        </is>
-      </c>
-      <c r="F302" t="inlineStr">
-        <is>
-          <t>Oceania</t>
-        </is>
-      </c>
-      <c r="G302" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 58df1aceb00ee7a435c85b831c9479bb0a64e72b
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G301"/>
+  <dimension ref="A1:G303"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5501,56 +5501,56 @@
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>QWJ</t>
+          <t>BOD</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Americana, Brazil</t>
+          <t>Bordeaux, France</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>-22.738</v>
+        <v>44.82946</v>
       </c>
       <c r="D166" t="n">
-        <v>-47.334</v>
+        <v>-0.58355</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>Americana</t>
+          <t>Bordeaux</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>ARI</t>
+          <t>QWJ</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Arica, Chile</t>
+          <t>Americana, Brazil</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>-18.348611</v>
+        <v>-22.738</v>
       </c>
       <c r="D167" t="n">
-        <v>-70.33888899999999</v>
+        <v>-47.334</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -5560,30 +5560,30 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>Arica</t>
+          <t>Americana</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>ASU</t>
+          <t>ARI</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Asunción, Paraguay</t>
+          <t>Arica, Chile</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>-25.2399997711</v>
+        <v>-18.348611</v>
       </c>
       <c r="D168" t="n">
-        <v>-57.5200004578</v>
+        <v>-70.33888899999999</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>PY</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -5593,30 +5593,30 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>Asunción</t>
+          <t>Arica</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>BEL</t>
+          <t>ASU</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Belém, Brazil</t>
+          <t>Asunción, Paraguay</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>-1.4563</v>
+        <v>-25.2399997711</v>
       </c>
       <c r="D169" t="n">
-        <v>-48.5013</v>
+        <v>-57.5200004578</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PY</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -5626,26 +5626,26 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>Belém</t>
+          <t>Asunción</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>CNF</t>
+          <t>BEL</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Belo Horizonte, Brazil</t>
+          <t>Belém, Brazil</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>-19.624444</v>
+        <v>-1.4563</v>
       </c>
       <c r="D170" t="n">
-        <v>-43.971944</v>
+        <v>-48.5013</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -5659,26 +5659,26 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>Belo Horizonte</t>
+          <t>Belém</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>BNU</t>
+          <t>CNF</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Blumenau, Brazil</t>
+          <t>Belo Horizonte, Brazil</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>-26.89245</v>
+        <v>-19.624444</v>
       </c>
       <c r="D171" t="n">
-        <v>-49.07696</v>
+        <v>-43.971944</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -5692,30 +5692,30 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Blumenau</t>
+          <t>Belo Horizonte</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>BOG</t>
+          <t>BNU</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Bogotá, Colombia</t>
+          <t>Blumenau, Brazil</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>4.70159</v>
+        <v>-26.89245</v>
       </c>
       <c r="D172" t="n">
-        <v>-74.1469</v>
+        <v>-49.07696</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -5725,30 +5725,30 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Blumenau</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>BSB</t>
+          <t>BOG</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Brasilia, Brazil</t>
+          <t>Bogotá, Colombia</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>-15.79824</v>
+        <v>4.70159</v>
       </c>
       <c r="D173" t="n">
-        <v>-47.90859</v>
+        <v>-74.1469</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -5758,30 +5758,30 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Brasilia</t>
+          <t>Bogotá</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>EZE</t>
+          <t>BSB</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Buenos Aires, Argentina</t>
+          <t>Brasilia, Brazil</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>-34.8222</v>
+        <v>-15.79824</v>
       </c>
       <c r="D174" t="n">
-        <v>-58.5358</v>
+        <v>-47.90859</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -5791,30 +5791,30 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>Buenos Aires</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>CFC</t>
+          <t>EZE</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Caçador, Brazil</t>
+          <t>Buenos Aires, Argentina</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>-26.7762</v>
+        <v>-34.8222</v>
       </c>
       <c r="D175" t="n">
-        <v>-51.0125</v>
+        <v>-58.5358</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -5824,26 +5824,26 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>Cacador</t>
+          <t>Buenos Aires</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>VCP</t>
+          <t>CFC</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Campinas, Brazil</t>
+          <t>Caçador, Brazil</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>-22.90662</v>
+        <v>-26.7762</v>
       </c>
       <c r="D176" t="n">
-        <v>-47.08576</v>
+        <v>-51.0125</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -5857,30 +5857,30 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>Campinas</t>
+          <t>Cacador</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>COR</t>
+          <t>VCP</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Córdoba, Argentina</t>
+          <t>Campinas, Brazil</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>-31.31</v>
+        <v>-22.90662</v>
       </c>
       <c r="D177" t="n">
-        <v>-64.208333</v>
+        <v>-47.08576</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -5890,30 +5890,30 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Campinas</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>CGB</t>
+          <t>COR</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Cuiabá, Brazil</t>
+          <t>Córdoba, Argentina</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>-15.59611</v>
+        <v>-31.31</v>
       </c>
       <c r="D178" t="n">
-        <v>-56.09667</v>
+        <v>-64.208333</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -5923,26 +5923,26 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>Cuiaba</t>
+          <t>Córdoba</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>CWB</t>
+          <t>CGB</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Curitiba, Brazil</t>
+          <t>Cuiabá, Brazil</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>-25.5284996033</v>
+        <v>-15.59611</v>
       </c>
       <c r="D179" t="n">
-        <v>-49.1758003235</v>
+        <v>-56.09667</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -5956,26 +5956,26 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>Curitiba</t>
+          <t>Cuiaba</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>FLN</t>
+          <t>CWB</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Florianopolis, Brazil</t>
+          <t>Curitiba, Brazil</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>-27.6702785492</v>
+        <v>-25.5284996033</v>
       </c>
       <c r="D180" t="n">
-        <v>-48.5525016785</v>
+        <v>-49.1758003235</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -5989,26 +5989,26 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>Florianopolis</t>
+          <t>Curitiba</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>FOR</t>
+          <t>FLN</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Fortaleza, Brazil</t>
+          <t>Florianopolis, Brazil</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>-3.7762799263</v>
+        <v>-27.6702785492</v>
       </c>
       <c r="D181" t="n">
-        <v>-38.5326004028</v>
+        <v>-48.5525016785</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -6022,30 +6022,30 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Florianopolis</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>GEO</t>
+          <t>FOR</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Georgetown, Guyana</t>
+          <t>Fortaleza, Brazil</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>6.825648</v>
+        <v>-3.7762799263</v>
       </c>
       <c r="D182" t="n">
-        <v>-58.163756</v>
+        <v>-38.5326004028</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>GY</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -6055,30 +6055,30 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>Georgetown</t>
+          <t>Fortaleza</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>GYN</t>
+          <t>GEO</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Goiânia, Brazil</t>
+          <t>Georgetown, Guyana</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>-16.69727</v>
+        <v>6.825648</v>
       </c>
       <c r="D183" t="n">
-        <v>-49.26851</v>
+        <v>-58.163756</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GY</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -6088,96 +6088,96 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>Goiania</t>
+          <t>Georgetown</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>GUA</t>
+          <t>GYN</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Guatemala City, Guatemala</t>
+          <t>Goiânia, Brazil</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>14.5832996368</v>
+        <v>-16.69727</v>
       </c>
       <c r="D184" t="n">
-        <v>-90.5274963379</v>
+        <v>-49.26851</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>GT</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>Guatemala City</t>
+          <t>Goiania</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>GYE</t>
+          <t>GUA</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Guayaquil, Ecuador</t>
+          <t>Guatemala City, Guatemala</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>-2.1894</v>
+        <v>14.5832996368</v>
       </c>
       <c r="D185" t="n">
-        <v>-79.8891</v>
+        <v>-90.5274963379</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>GT</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>Guayaquil</t>
+          <t>Guatemala City</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>ITJ</t>
+          <t>GYE</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Itajaí, Brazil</t>
+          <t>Guayaquil, Ecuador</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>-27.6116676331</v>
+        <v>-2.1894</v>
       </c>
       <c r="D186" t="n">
-        <v>-48.6727790833</v>
+        <v>-79.8891</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -6187,26 +6187,26 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>Itajai</t>
+          <t>Guayaquil</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
         <is>
-          <t>JOI</t>
+          <t>ITJ</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Joinville, Brazil</t>
+          <t>Itajaí, Brazil</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>-26.304408</v>
+        <v>-27.6116676331</v>
       </c>
       <c r="D187" t="n">
-        <v>-48.846383</v>
+        <v>-48.6727790833</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -6220,26 +6220,26 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>Joinville</t>
+          <t>Itajai</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
         <is>
-          <t>JDO</t>
+          <t>JOI</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte, Brazil</t>
+          <t>Joinville, Brazil</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>-7.2242</v>
+        <v>-26.304408</v>
       </c>
       <c r="D188" t="n">
-        <v>-39.313</v>
+        <v>-48.846383</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -6253,30 +6253,30 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte</t>
+          <t>Joinville</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>LIM</t>
+          <t>JDO</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Lima, Peru</t>
+          <t>Juazeiro do Norte, Brazil</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>-12.021900177</v>
+        <v>-7.2242</v>
       </c>
       <c r="D189" t="n">
-        <v>-77.1143035889</v>
+        <v>-39.313</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -6286,30 +6286,30 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>Lima</t>
+          <t>Juazeiro do Norte</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
         <is>
-          <t>MAO</t>
+          <t>LIM</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Manaus, Brazil</t>
+          <t>Lima, Peru</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>-3.11286</v>
+        <v>-12.021900177</v>
       </c>
       <c r="D190" t="n">
-        <v>-60.01949</v>
+        <v>-77.1143035889</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -6319,30 +6319,30 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>Manaus</t>
+          <t>Lima</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
         <is>
-          <t>MDE</t>
+          <t>MAO</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Medellín, Colombia</t>
+          <t>Manaus, Brazil</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>6.16454</v>
+        <v>-3.11286</v>
       </c>
       <c r="D191" t="n">
-        <v>-75.42310000000001</v>
+        <v>-60.01949</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -6352,30 +6352,30 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>Medellín</t>
+          <t>Manaus</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
         <is>
-          <t>NQN</t>
+          <t>MDE</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Neuquén, Argentina</t>
+          <t>Medellín, Colombia</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>-38.9490013123</v>
+        <v>6.16454</v>
       </c>
       <c r="D192" t="n">
-        <v>-68.1557006836</v>
+        <v>-75.42310000000001</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -6385,30 +6385,30 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>Neuquen</t>
+          <t>Medellín</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
         <is>
-          <t>PTY</t>
+          <t>NQN</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Panama City, Panama</t>
+          <t>Neuquén, Argentina</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>9.0713596344</v>
+        <v>-38.9490013123</v>
       </c>
       <c r="D193" t="n">
-        <v>-79.3834991455</v>
+        <v>-68.1557006836</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -6418,30 +6418,30 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>Panama City</t>
+          <t>Neuquen</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
         <is>
-          <t>PBM</t>
+          <t>PTY</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Paramaribo, Suriname</t>
+          <t>Panama City, Panama</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>5.452831</v>
+        <v>9.0713596344</v>
       </c>
       <c r="D194" t="n">
-        <v>-55.187783</v>
+        <v>-79.3834991455</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>SR</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -6451,30 +6451,30 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>Paramaribo</t>
+          <t>Panama City</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
         <is>
-          <t>POA</t>
+          <t>PBM</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Porto Alegre, Brazil</t>
+          <t>Paramaribo, Suriname</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>-29.9944000244</v>
+        <v>5.452831</v>
       </c>
       <c r="D195" t="n">
-        <v>-51.1713981628</v>
+        <v>-55.187783</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>SR</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -6484,30 +6484,30 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>Porto Alegre</t>
+          <t>Paramaribo</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
         <is>
-          <t>UIO</t>
+          <t>POA</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Quito, Ecuador</t>
+          <t>Porto Alegre, Brazil</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>-0.1291666667</v>
+        <v>-29.9944000244</v>
       </c>
       <c r="D196" t="n">
-        <v>-78.3575</v>
+        <v>-51.1713981628</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -6517,30 +6517,30 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>Quito</t>
+          <t>Porto Alegre</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>UIO</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Recife, Brazil</t>
+          <t>Quito, Ecuador</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>-8.126489639300001</v>
+        <v>-0.1291666667</v>
       </c>
       <c r="D197" t="n">
-        <v>-34.9235992432</v>
+        <v>-78.3575</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -6550,26 +6550,26 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>Quito</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>REC</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Ribeirao Preto, Brazil</t>
+          <t>Recife, Brazil</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>-21.1363887787</v>
+        <v>-8.126489639300001</v>
       </c>
       <c r="D198" t="n">
-        <v>-47.7766685486</v>
+        <v>-34.9235992432</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -6583,26 +6583,26 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>Ribeirao Preto</t>
+          <t>Recife</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>GIG</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Rio de Janeiro, Brazil</t>
+          <t>Ribeirao Preto, Brazil</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>-22.8099994659</v>
+        <v>-21.1363887787</v>
       </c>
       <c r="D199" t="n">
-        <v>-43.2505569458</v>
+        <v>-47.7766685486</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -6616,26 +6616,26 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>Ribeirao Preto</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>GIG</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Salvador, Brazil</t>
+          <t>Rio de Janeiro, Brazil</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>-12.9086112976</v>
+        <v>-22.8099994659</v>
       </c>
       <c r="D200" t="n">
-        <v>-38.3224983215</v>
+        <v>-43.2505569458</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -6649,30 +6649,30 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Salvador</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>San José, Costa Rica</t>
+          <t>Salvador, Brazil</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>9.9938602448</v>
+        <v>-12.9086112976</v>
       </c>
       <c r="D201" t="n">
-        <v>-84.2088012695</v>
+        <v>-38.3224983215</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -6682,30 +6682,30 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Santiago, Chile</t>
+          <t>San José, Costa Rica</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>-33.3930015564</v>
+        <v>9.9938602448</v>
       </c>
       <c r="D202" t="n">
-        <v>-70.7857971191</v>
+        <v>-84.2088012695</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -6715,92 +6715,92 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>San José</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>SDQ</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Santo Domingo, Dominican Republic</t>
+          <t>Santiago, Chile</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>18.4297008514</v>
+        <v>-33.3930015564</v>
       </c>
       <c r="D203" t="n">
-        <v>-69.6688995361</v>
+        <v>-70.7857971191</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>DO</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Santo Domingo</t>
+          <t>Santiago</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SDQ</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>São José do Rio Preto, Brazil</t>
+          <t>Santo Domingo, Dominican Republic</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>-20.807157</v>
+        <v>18.4297008514</v>
       </c>
       <c r="D204" t="n">
-        <v>-49.378994</v>
+        <v>-69.6688995361</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>Santo Domingo</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>SJK</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>São José dos Campos, Brazil</t>
+          <t>São José do Rio Preto, Brazil</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>-23.1791</v>
+        <v>-20.807157</v>
       </c>
       <c r="D205" t="n">
-        <v>-45.8872</v>
+        <v>-49.378994</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -6814,26 +6814,26 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>São José dos Campos</t>
+          <t>São José do Rio Preto</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SJK</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>São José dos Campos, Brazil</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>-23.4355564117</v>
+        <v>-23.1791</v>
       </c>
       <c r="D206" t="n">
-        <v>-46.4730567932</v>
+        <v>-45.8872</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -6847,26 +6847,26 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>São José dos Campos</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>-23.54389</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="D207" t="n">
-        <v>-46.63445</v>
+        <v>-46.4730567932</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -6880,30 +6880,30 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>12.007116</v>
+        <v>-23.54389</v>
       </c>
       <c r="D208" t="n">
-        <v>-61.7882288</v>
+        <v>-46.63445</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -6913,30 +6913,30 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Sorocaba</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>14.0608</v>
+        <v>12.007116</v>
       </c>
       <c r="D209" t="n">
-        <v>-87.21720000000001</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -6946,30 +6946,30 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>NVT</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Timbó, Brazil</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>-26.8251</v>
+        <v>14.0608</v>
       </c>
       <c r="D210" t="n">
-        <v>-49.2695</v>
+        <v>-87.21720000000001</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -6979,26 +6979,26 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Timbo</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>NVT</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Timbó, Brazil</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>-18.8836116791</v>
+        <v>-26.8251</v>
       </c>
       <c r="D211" t="n">
-        <v>-48.225276947</v>
+        <v>-49.2695</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -7012,26 +7012,26 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Timbo</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>VIX</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Vitoria, Brazil</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>-20.64871</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="D212" t="n">
-        <v>-41.90857</v>
+        <v>-48.225276947</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -7045,30 +7045,30 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>VIX</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Vitoria, Brazil</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>12.1888999939</v>
+        <v>-20.64871</v>
       </c>
       <c r="D213" t="n">
-        <v>-68.95980072019999</v>
+        <v>-41.90857</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -7078,30 +7078,30 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Vitoria</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>CAW</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes, Brazil</t>
+          <t>Willemstad, Curaçao</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>-21.698299408</v>
+        <v>12.1888999939</v>
       </c>
       <c r="D214" t="n">
-        <v>-41.301700592</v>
+        <v>-68.95980072019999</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -7111,63 +7111,63 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes</t>
+          <t>Willemstad</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>CAW</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Campos dos Goytacazes, Brazil</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>31.7226009369</v>
+        <v>-21.698299408</v>
       </c>
       <c r="D215" t="n">
-        <v>35.9931983948</v>
+        <v>-41.301700592</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Campos dos Goytacazes</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D216" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -7177,30 +7177,30 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D217" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7210,30 +7210,30 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D218" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -7243,30 +7243,30 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D219" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7276,30 +7276,30 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D220" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7309,30 +7309,30 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D221" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -7342,30 +7342,30 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="D222" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7375,30 +7375,30 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="D223" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7408,30 +7408,30 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D224" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7441,30 +7441,30 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="D225" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -7474,30 +7474,30 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>21.679599762</v>
+        <v>32.78492</v>
       </c>
       <c r="D226" t="n">
-        <v>39.15650177</v>
+        <v>34.96069</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -7507,30 +7507,30 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>29.226600647</v>
+        <v>21.679599762</v>
       </c>
       <c r="D227" t="n">
-        <v>47.9688987732</v>
+        <v>39.15650177</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -7540,30 +7540,30 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D228" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -7573,30 +7573,30 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D229" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7606,30 +7606,30 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D230" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -7639,26 +7639,26 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D231" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -7672,30 +7672,30 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D232" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -7705,30 +7705,30 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D233" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -7738,30 +7738,30 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>35.5668</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D234" t="n">
-        <v>45.4161</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -7771,30 +7771,30 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>32.0113983154</v>
+        <v>35.5668</v>
       </c>
       <c r="D235" t="n">
-        <v>34.8866996765</v>
+        <v>45.4161</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -7804,59 +7804,59 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>38.94449997</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D236" t="n">
-        <v>-77.45580292</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="D237" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -7870,26 +7870,26 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D238" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -7903,26 +7903,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D239" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7936,30 +7936,30 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D240" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -7969,30 +7969,30 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D241" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -8002,26 +8002,26 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D242" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -8035,26 +8035,26 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D243" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -8068,26 +8068,26 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D244" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -8101,26 +8101,26 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D245" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -8134,26 +8134,26 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D246" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -8167,26 +8167,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D247" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8200,26 +8200,26 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D248" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8233,26 +8233,26 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D249" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8266,26 +8266,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D250" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8299,26 +8299,26 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D251" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8332,26 +8332,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D252" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8365,26 +8365,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D253" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8398,26 +8398,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D254" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8431,26 +8431,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D255" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8464,30 +8464,30 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D256" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -8497,30 +8497,30 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D257" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -8530,26 +8530,26 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D258" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8563,26 +8563,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D259" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8596,30 +8596,30 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D260" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -8629,30 +8629,30 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D261" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -8662,26 +8662,26 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D262" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8695,26 +8695,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D263" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8728,26 +8728,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D264" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8761,30 +8761,30 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D265" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -8794,30 +8794,30 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D266" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -8827,26 +8827,26 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D267" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -8860,26 +8860,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D268" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8893,26 +8893,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D269" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8926,30 +8926,30 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D270" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -8959,30 +8959,30 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D271" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -8992,26 +8992,26 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D272" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -9025,26 +9025,26 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D273" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -9058,26 +9058,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D274" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -9091,26 +9091,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D275" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9124,30 +9124,30 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D276" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -9157,30 +9157,30 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D277" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9190,26 +9190,26 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D278" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -9223,26 +9223,26 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D279" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -9256,26 +9256,26 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D280" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -9289,30 +9289,30 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>43.6772003174</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D281" t="n">
-        <v>-79.63059997560001</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -9322,26 +9322,26 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D282" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -9355,26 +9355,26 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D283" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -9388,30 +9388,30 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D284" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -9421,30 +9421,30 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D285" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -9454,30 +9454,30 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>44.8081</v>
+        <v>17.9951</v>
       </c>
       <c r="D286" t="n">
-        <v>-68.795</v>
+        <v>-76.7846</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9487,26 +9487,26 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>30.1975</v>
+        <v>44.8081</v>
       </c>
       <c r="D287" t="n">
-        <v>-97.6664</v>
+        <v>-68.795</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -9520,26 +9520,26 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>35.0844</v>
+        <v>30.1975</v>
       </c>
       <c r="D288" t="n">
-        <v>-106.6504</v>
+        <v>-97.6664</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -9553,30 +9553,30 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>20.5217990875</v>
+        <v>35.0844</v>
       </c>
       <c r="D289" t="n">
-        <v>-103.3109970093</v>
+        <v>-106.6504</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -9586,92 +9586,92 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>-34.9431729</v>
+        <v>20.5217990875</v>
       </c>
       <c r="D290" t="n">
-        <v>138.5335637</v>
+        <v>-103.3109970093</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Guadalajara</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>-37.0080986023</v>
+        <v>29.429461</v>
       </c>
       <c r="D291" t="n">
-        <v>174.792007446</v>
+        <v>-98.487061</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>San Antonio</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>-27.3841991425</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D292" t="n">
-        <v>153.117004394</v>
+        <v>138.5335637</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -9685,30 +9685,30 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>-35.3069000244</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D293" t="n">
-        <v>149.1950073242</v>
+        <v>174.792007446</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -9718,30 +9718,30 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>-43.4893989563</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D294" t="n">
-        <v>172.5319976807</v>
+        <v>153.117004394</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -9751,63 +9751,63 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>13.4834003448</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D295" t="n">
-        <v>144.796005249</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>-42.883209</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D296" t="n">
-        <v>147.331665</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
@@ -9817,63 +9817,63 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>-37.6733016968</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D297" t="n">
-        <v>144.843002319</v>
+        <v>144.796005249</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>-22.0146007538</v>
+        <v>-42.883209</v>
       </c>
       <c r="D298" t="n">
-        <v>166.212997436</v>
+        <v>147.331665</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -9883,26 +9883,26 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>-31.9402999878</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D299" t="n">
-        <v>115.967002869</v>
+        <v>144.843002319</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -9916,30 +9916,30 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>-33.9460983276</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D300" t="n">
-        <v>151.177001953</v>
+        <v>166.212997436</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -9949,38 +9949,104 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
+          <t>PER</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>Perth, WA, Australia</t>
+        </is>
+      </c>
+      <c r="C301" t="n">
+        <v>-31.9402999878</v>
+      </c>
+      <c r="D301" t="n">
+        <v>115.967002869</v>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G301" t="inlineStr">
+        <is>
+          <t>Perth</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="1" t="inlineStr">
+        <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Sydney, NSW, Australia</t>
+        </is>
+      </c>
+      <c r="C302" t="n">
+        <v>-33.9460983276</v>
+      </c>
+      <c r="D302" t="n">
+        <v>151.177001953</v>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G302" t="inlineStr">
+        <is>
+          <t>Sydney</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="1" t="inlineStr">
+        <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="B301" t="inlineStr">
+      <c r="B303" t="inlineStr">
         <is>
           <t>Tahiti, French Polynesia</t>
         </is>
       </c>
-      <c r="C301" t="n">
+      <c r="C303" t="n">
         <v>-17.5536994934</v>
       </c>
-      <c r="D301" t="n">
+      <c r="D303" t="n">
         <v>-149.606994629</v>
       </c>
-      <c r="E301" t="inlineStr">
+      <c r="E303" t="inlineStr">
         <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="F301" t="inlineStr">
+      <c r="F303" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G301" t="inlineStr">
+      <c r="G303" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 9bf8990f8954b28459aecc05cc2d0b71f36e0852
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -3436,12 +3436,12 @@
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>TYN</t>
+          <t>WHU</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Datong, China</t>
+          <t>Wuhu, China</t>
         </is>
       </c>
       <c r="C101" t="inlineStr"/>
@@ -3453,12 +3453,12 @@
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>WHU</t>
+          <t>HYN</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Wuhu, China</t>
+          <t>Taizhou, China</t>
         </is>
       </c>
       <c r="C102" t="inlineStr"/>
@@ -3470,90 +3470,106 @@
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>HYN</t>
+          <t>COK</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Taizhou, China</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr"/>
-      <c r="D103" t="inlineStr"/>
-      <c r="E103" t="inlineStr"/>
-      <c r="F103" t="inlineStr"/>
-      <c r="G103" t="inlineStr"/>
+          <t>Kochi, India</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>9.9312</v>
+      </c>
+      <c r="D103" t="n">
+        <v>76.26730000000001</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Asia Pacific</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>Kochi</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>COK</t>
+          <t>XMN</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Kochi, India</t>
-        </is>
-      </c>
-      <c r="C104" t="n">
-        <v>9.9312</v>
-      </c>
-      <c r="D104" t="n">
-        <v>76.26730000000001</v>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>Asia Pacific</t>
-        </is>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>Kochi</t>
-        </is>
-      </c>
+          <t>Xiamen, China</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr"/>
+      <c r="E104" t="inlineStr"/>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>XMN</t>
+          <t>DPS</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Xiamen, China</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr"/>
-      <c r="D105" t="inlineStr"/>
-      <c r="E105" t="inlineStr"/>
-      <c r="F105" t="inlineStr"/>
-      <c r="G105" t="inlineStr"/>
+          <t>Denpasar, Indonesia</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>-8.748169899000001</v>
+      </c>
+      <c r="D105" t="n">
+        <v>115.1669998169</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Asia Pacific</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>Denpasar</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>DPS</t>
+          <t>CNN</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Denpasar, Indonesia</t>
+          <t>Kannur, India</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>-8.748169899000001</v>
+        <v>11.915858</v>
       </c>
       <c r="D106" t="n">
-        <v>115.1669998169</v>
+        <v>75.55094</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -3563,52 +3579,36 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>Denpasar</t>
+          <t>Kannur</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>CNN</t>
+          <t>SZX</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Kannur, India</t>
-        </is>
-      </c>
-      <c r="C107" t="n">
-        <v>11.915858</v>
-      </c>
-      <c r="D107" t="n">
-        <v>75.55094</v>
-      </c>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>Asia Pacific</t>
-        </is>
-      </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>Kannur</t>
-        </is>
-      </c>
+          <t>Shenzhen, China</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr"/>
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="inlineStr"/>
+      <c r="G107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>SZX</t>
+          <t>KWE</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Shenzhen, China</t>
+          <t>Guiyang, China</t>
         </is>
       </c>
       <c r="C108" t="inlineStr"/>

</xml_diff>

<commit_message>
update generated data Triggered by 2a001073886699d8eefd1980be4b2c76048e6f8e
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H304"/>
+  <dimension ref="A1:H305"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8148,66 +8148,66 @@
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>XAP</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Chapeco, Brazil</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>XAP</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>31.7226009369</v>
+        <v>-27.1341991425</v>
       </c>
       <c r="E217" t="n">
-        <v>35.9931983948</v>
+        <v>-52.6566009521</v>
       </c>
       <c r="F217" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="H217" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Chapeco</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="E218" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="G218" t="inlineStr">
@@ -8217,35 +8217,35 @@
       </c>
       <c r="H218" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="D219" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="E219" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="G219" t="inlineStr">
@@ -8255,35 +8255,35 @@
       </c>
       <c r="H219" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="E220" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="G220" t="inlineStr">
@@ -8293,35 +8293,35 @@
       </c>
       <c r="H220" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="E221" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="G221" t="inlineStr">
@@ -8331,35 +8331,35 @@
       </c>
       <c r="H221" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="E222" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="G222" t="inlineStr">
@@ -8369,35 +8369,35 @@
       </c>
       <c r="H222" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="E223" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="F223" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="G223" t="inlineStr">
@@ -8407,35 +8407,35 @@
       </c>
       <c r="H223" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="E224" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="F224" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="G224" t="inlineStr">
@@ -8445,35 +8445,35 @@
       </c>
       <c r="H224" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="E225" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="G225" t="inlineStr">
@@ -8483,35 +8483,35 @@
       </c>
       <c r="H225" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="E226" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="G226" t="inlineStr">
@@ -8521,35 +8521,35 @@
       </c>
       <c r="H226" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="E227" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="G227" t="inlineStr">
@@ -8559,35 +8559,35 @@
       </c>
       <c r="H227" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>21.679599762</v>
+        <v>32.78492</v>
       </c>
       <c r="E228" t="n">
-        <v>39.15650177</v>
+        <v>34.96069</v>
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="G228" t="inlineStr">
@@ -8597,35 +8597,35 @@
       </c>
       <c r="H228" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>29.226600647</v>
+        <v>21.679599762</v>
       </c>
       <c r="E229" t="n">
-        <v>47.9688987732</v>
+        <v>39.15650177</v>
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="G229" t="inlineStr">
@@ -8635,35 +8635,35 @@
       </c>
       <c r="H229" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="E230" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="F230" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="G230" t="inlineStr">
@@ -8673,35 +8673,35 @@
       </c>
       <c r="H230" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="E231" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="G231" t="inlineStr">
@@ -8711,35 +8711,35 @@
       </c>
       <c r="H231" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="E232" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="G232" t="inlineStr">
@@ -8749,31 +8749,31 @@
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="E233" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="F233" t="inlineStr">
         <is>
@@ -8787,35 +8787,35 @@
       </c>
       <c r="H233" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="E234" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="F234" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="G234" t="inlineStr">
@@ -8825,35 +8825,35 @@
       </c>
       <c r="H234" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="E235" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="G235" t="inlineStr">
@@ -8863,35 +8863,35 @@
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>35.5668</v>
+        <v>24.9575996399</v>
       </c>
       <c r="E236" t="n">
-        <v>45.4161</v>
+        <v>46.6987991333</v>
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="G236" t="inlineStr">
@@ -8901,35 +8901,35 @@
       </c>
       <c r="H236" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>32.0113983154</v>
+        <v>35.5668</v>
       </c>
       <c r="E237" t="n">
-        <v>34.8866996765</v>
+        <v>45.4161</v>
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="G237" t="inlineStr">
@@ -8939,69 +8939,69 @@
       </c>
       <c r="H237" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>38.94449997</v>
+        <v>32.0113983154</v>
       </c>
       <c r="E238" t="n">
-        <v>-77.45580292</v>
+        <v>34.8866996765</v>
       </c>
       <c r="F238" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="H238" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="E239" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="F239" t="inlineStr">
         <is>
@@ -9015,31 +9015,31 @@
       </c>
       <c r="H239" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="E240" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="F240" t="inlineStr">
         <is>
@@ -9053,31 +9053,31 @@
       </c>
       <c r="H240" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="E241" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="F241" t="inlineStr">
         <is>
@@ -9091,35 +9091,35 @@
       </c>
       <c r="H241" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="E242" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G242" t="inlineStr">
@@ -9129,35 +9129,35 @@
       </c>
       <c r="H242" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="E243" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="F243" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G243" t="inlineStr">
@@ -9167,31 +9167,31 @@
       </c>
       <c r="H243" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="E244" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="F244" t="inlineStr">
         <is>
@@ -9205,31 +9205,31 @@
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="E245" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="F245" t="inlineStr">
         <is>
@@ -9243,31 +9243,31 @@
       </c>
       <c r="H245" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="E246" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="F246" t="inlineStr">
         <is>
@@ -9281,31 +9281,31 @@
       </c>
       <c r="H246" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="E247" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="F247" t="inlineStr">
         <is>
@@ -9319,31 +9319,31 @@
       </c>
       <c r="H247" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="D248" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="E248" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="F248" t="inlineStr">
         <is>
@@ -9357,31 +9357,31 @@
       </c>
       <c r="H248" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="E249" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="F249" t="inlineStr">
         <is>
@@ -9395,31 +9395,31 @@
       </c>
       <c r="H249" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="E250" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="F250" t="inlineStr">
         <is>
@@ -9433,31 +9433,31 @@
       </c>
       <c r="H250" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="E251" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="F251" t="inlineStr">
         <is>
@@ -9471,31 +9471,31 @@
       </c>
       <c r="H251" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="E252" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="F252" t="inlineStr">
         <is>
@@ -9509,31 +9509,31 @@
       </c>
       <c r="H252" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="E253" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="F253" t="inlineStr">
         <is>
@@ -9547,31 +9547,31 @@
       </c>
       <c r="H253" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="D254" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="E254" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="F254" t="inlineStr">
         <is>
@@ -9585,31 +9585,31 @@
       </c>
       <c r="H254" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="D255" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="E255" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="F255" t="inlineStr">
         <is>
@@ -9623,31 +9623,31 @@
       </c>
       <c r="H255" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="D256" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="E256" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="F256" t="inlineStr">
         <is>
@@ -9661,31 +9661,31 @@
       </c>
       <c r="H256" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="E257" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="F257" t="inlineStr">
         <is>
@@ -9699,35 +9699,35 @@
       </c>
       <c r="H257" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="E258" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="F258" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G258" t="inlineStr">
@@ -9737,35 +9737,35 @@
       </c>
       <c r="H258" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="E259" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="F259" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G259" t="inlineStr">
@@ -9775,31 +9775,31 @@
       </c>
       <c r="H259" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="E260" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="F260" t="inlineStr">
         <is>
@@ -9813,31 +9813,31 @@
       </c>
       <c r="H260" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="E261" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="F261" t="inlineStr">
         <is>
@@ -9851,35 +9851,35 @@
       </c>
       <c r="H261" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="E262" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G262" t="inlineStr">
@@ -9889,35 +9889,35 @@
       </c>
       <c r="H262" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="E263" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="F263" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G263" t="inlineStr">
@@ -9927,31 +9927,31 @@
       </c>
       <c r="H263" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="E264" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="F264" t="inlineStr">
         <is>
@@ -9965,31 +9965,31 @@
       </c>
       <c r="H264" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="E265" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="F265" t="inlineStr">
         <is>
@@ -10003,31 +10003,31 @@
       </c>
       <c r="H265" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="E266" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="F266" t="inlineStr">
         <is>
@@ -10041,35 +10041,35 @@
       </c>
       <c r="H266" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="E267" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="F267" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G267" t="inlineStr">
@@ -10079,35 +10079,35 @@
       </c>
       <c r="H267" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="E268" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G268" t="inlineStr">
@@ -10117,31 +10117,31 @@
       </c>
       <c r="H268" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="E269" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="F269" t="inlineStr">
         <is>
@@ -10155,31 +10155,31 @@
       </c>
       <c r="H269" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="E270" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="F270" t="inlineStr">
         <is>
@@ -10193,31 +10193,31 @@
       </c>
       <c r="H270" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="E271" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="F271" t="inlineStr">
         <is>
@@ -10231,35 +10231,35 @@
       </c>
       <c r="H271" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="E272" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G272" t="inlineStr">
@@ -10269,35 +10269,35 @@
       </c>
       <c r="H272" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="D273" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="E273" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G273" t="inlineStr">
@@ -10307,31 +10307,31 @@
       </c>
       <c r="H273" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="E274" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="F274" t="inlineStr">
         <is>
@@ -10345,31 +10345,31 @@
       </c>
       <c r="H274" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="E275" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="F275" t="inlineStr">
         <is>
@@ -10383,31 +10383,31 @@
       </c>
       <c r="H275" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="E276" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="F276" t="inlineStr">
         <is>
@@ -10421,31 +10421,31 @@
       </c>
       <c r="H276" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="E277" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="F277" t="inlineStr">
         <is>
@@ -10459,35 +10459,35 @@
       </c>
       <c r="H277" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="E278" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G278" t="inlineStr">
@@ -10497,35 +10497,35 @@
       </c>
       <c r="H278" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="E279" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G279" t="inlineStr">
@@ -10535,31 +10535,31 @@
       </c>
       <c r="H279" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="E280" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
       <c r="F280" t="inlineStr">
         <is>
@@ -10573,31 +10573,31 @@
       </c>
       <c r="H280" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="E281" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="F281" t="inlineStr">
         <is>
@@ -10611,31 +10611,31 @@
       </c>
       <c r="H281" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="E282" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="F282" t="inlineStr">
         <is>
@@ -10649,35 +10649,35 @@
       </c>
       <c r="H282" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>43.6772003174</v>
+        <v>30.3964996338</v>
       </c>
       <c r="E283" t="n">
-        <v>-79.63059997560001</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G283" t="inlineStr">
@@ -10687,31 +10687,31 @@
       </c>
       <c r="H283" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="E284" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="F284" t="inlineStr">
         <is>
@@ -10725,31 +10725,31 @@
       </c>
       <c r="H284" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="E285" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="F285" t="inlineStr">
         <is>
@@ -10763,35 +10763,35 @@
       </c>
       <c r="H285" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="E286" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G286" t="inlineStr">
@@ -10801,35 +10801,35 @@
       </c>
       <c r="H286" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="E287" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G287" t="inlineStr">
@@ -10839,35 +10839,35 @@
       </c>
       <c r="H287" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>44.8081</v>
+        <v>17.9951</v>
       </c>
       <c r="E288" t="n">
-        <v>-68.795</v>
+        <v>-76.7846</v>
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="G288" t="inlineStr">
@@ -10877,31 +10877,31 @@
       </c>
       <c r="H288" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>30.1975</v>
+        <v>44.8081</v>
       </c>
       <c r="E289" t="n">
-        <v>-97.6664</v>
+        <v>-68.795</v>
       </c>
       <c r="F289" t="inlineStr">
         <is>
@@ -10915,31 +10915,31 @@
       </c>
       <c r="H289" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>35.0844</v>
+        <v>30.1975</v>
       </c>
       <c r="E290" t="n">
-        <v>-106.6504</v>
+        <v>-97.6664</v>
       </c>
       <c r="F290" t="inlineStr">
         <is>
@@ -10953,35 +10953,35 @@
       </c>
       <c r="H290" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>20.5217990875</v>
+        <v>35.0844</v>
       </c>
       <c r="E291" t="n">
-        <v>-103.3109970093</v>
+        <v>-106.6504</v>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G291" t="inlineStr">
@@ -10991,35 +10991,35 @@
       </c>
       <c r="H291" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>29.429461</v>
+        <v>20.5217990875</v>
       </c>
       <c r="E292" t="n">
-        <v>-98.487061</v>
+        <v>-103.3109970093</v>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G292" t="inlineStr">
@@ -11029,73 +11029,73 @@
       </c>
       <c r="H292" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Guadalajara</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>-34.9431729</v>
+        <v>29.429461</v>
       </c>
       <c r="E293" t="n">
-        <v>138.5335637</v>
+        <v>-98.487061</v>
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="H293" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>San Antonio</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="E294" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="G294" t="inlineStr">
@@ -11105,35 +11105,35 @@
       </c>
       <c r="H294" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="E295" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
@@ -11143,31 +11143,31 @@
       </c>
       <c r="H295" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="E296" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="F296" t="inlineStr">
         <is>
@@ -11181,35 +11181,35 @@
       </c>
       <c r="H296" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="E297" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="G297" t="inlineStr">
@@ -11219,107 +11219,107 @@
       </c>
       <c r="H297" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="E298" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="H298" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="E299" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="H299" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="E300" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="F300" t="inlineStr">
         <is>
@@ -11333,35 +11333,35 @@
       </c>
       <c r="H300" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="E301" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="G301" t="inlineStr">
@@ -11371,35 +11371,35 @@
       </c>
       <c r="H301" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="E302" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="G302" t="inlineStr">
@@ -11409,31 +11409,31 @@
       </c>
       <c r="H302" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="E303" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="F303" t="inlineStr">
         <is>
@@ -11447,43 +11447,81 @@
       </c>
       <c r="H303" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Sydney, NSW, Australia</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="D304" t="n">
+        <v>-33.9460983276</v>
+      </c>
+      <c r="E304" t="n">
+        <v>151.177001953</v>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="G304" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="H304" t="inlineStr">
+        <is>
+          <t>Sydney</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="1" t="inlineStr">
+        <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="B304" t="inlineStr">
+      <c r="B305" t="inlineStr">
         <is>
           <t>Tahiti, French Polynesia</t>
         </is>
       </c>
-      <c r="C304" t="inlineStr">
+      <c r="C305" t="inlineStr">
         <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="D304" t="n">
+      <c r="D305" t="n">
         <v>-17.5536994934</v>
       </c>
-      <c r="E304" t="n">
+      <c r="E305" t="n">
         <v>-149.606994629</v>
       </c>
-      <c r="F304" t="inlineStr">
+      <c r="F305" t="inlineStr">
         <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="G304" t="inlineStr">
+      <c r="G305" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="H304" t="inlineStr">
+      <c r="H305" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by a1a56ab4e7241714c2391fd4c3e076b2b86e2c8a
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H306"/>
+  <dimension ref="A1:H307"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11092,66 +11092,66 @@
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>-34.9431729</v>
+        <v>41.50069</v>
       </c>
       <c r="E295" t="n">
-        <v>138.5335637</v>
+        <v>-81.68411999999999</v>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="H295" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Cleveland</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="E296" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="G296" t="inlineStr">
@@ -11161,35 +11161,35 @@
       </c>
       <c r="H296" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="E297" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="G297" t="inlineStr">
@@ -11199,31 +11199,31 @@
       </c>
       <c r="H297" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="E298" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="F298" t="inlineStr">
         <is>
@@ -11237,35 +11237,35 @@
       </c>
       <c r="H298" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="E299" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="G299" t="inlineStr">
@@ -11275,107 +11275,107 @@
       </c>
       <c r="H299" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="E300" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="H300" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="E301" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="H301" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="E302" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="F302" t="inlineStr">
         <is>
@@ -11389,35 +11389,35 @@
       </c>
       <c r="H302" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="E303" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="G303" t="inlineStr">
@@ -11427,35 +11427,35 @@
       </c>
       <c r="H303" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="E304" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="G304" t="inlineStr">
@@ -11465,31 +11465,31 @@
       </c>
       <c r="H304" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="E305" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="F305" t="inlineStr">
         <is>
@@ -11503,43 +11503,81 @@
       </c>
       <c r="H305" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Sydney, NSW, Australia</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="D306" t="n">
+        <v>-33.9460983276</v>
+      </c>
+      <c r="E306" t="n">
+        <v>151.177001953</v>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="G306" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="H306" t="inlineStr">
+        <is>
+          <t>Sydney</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="1" t="inlineStr">
+        <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="B306" t="inlineStr">
+      <c r="B307" t="inlineStr">
         <is>
           <t>Tahiti, French Polynesia</t>
         </is>
       </c>
-      <c r="C306" t="inlineStr">
+      <c r="C307" t="inlineStr">
         <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="D306" t="n">
+      <c r="D307" t="n">
         <v>-17.5536994934</v>
       </c>
-      <c r="E306" t="n">
+      <c r="E307" t="n">
         <v>-149.606994629</v>
       </c>
-      <c r="F306" t="inlineStr">
+      <c r="F307" t="inlineStr">
         <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="G306" t="inlineStr">
+      <c r="G307" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="H306" t="inlineStr">
+      <c r="H307" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 0e04a5f484b7479db6f43e2ba4a2ab4fc69c67c9
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H310"/>
+  <dimension ref="A1:H311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11204,66 +11204,66 @@
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>-34.9431729</v>
+        <v>35.93543</v>
       </c>
       <c r="E299" t="n">
-        <v>138.5335637</v>
+        <v>-78.88075000000001</v>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="H299" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Durham</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="E300" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="G300" t="inlineStr">
@@ -11273,35 +11273,35 @@
       </c>
       <c r="H300" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="E301" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="G301" t="inlineStr">
@@ -11311,31 +11311,31 @@
       </c>
       <c r="H301" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="E302" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="F302" t="inlineStr">
         <is>
@@ -11349,35 +11349,35 @@
       </c>
       <c r="H302" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="E303" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="G303" t="inlineStr">
@@ -11387,107 +11387,107 @@
       </c>
       <c r="H303" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="E304" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="H304" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="E305" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="H305" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="E306" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="F306" t="inlineStr">
         <is>
@@ -11501,35 +11501,35 @@
       </c>
       <c r="H306" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="E307" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="G307" t="inlineStr">
@@ -11539,35 +11539,35 @@
       </c>
       <c r="H307" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="E308" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="G308" t="inlineStr">
@@ -11577,31 +11577,31 @@
       </c>
       <c r="H308" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="E309" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="F309" t="inlineStr">
         <is>
@@ -11615,43 +11615,81 @@
       </c>
       <c r="H309" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Sydney, NSW, Australia</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>-33.9460983276</v>
+      </c>
+      <c r="E310" t="n">
+        <v>151.177001953</v>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="G310" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="H310" t="inlineStr">
+        <is>
+          <t>Sydney</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="inlineStr">
+        <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="B310" t="inlineStr">
+      <c r="B311" t="inlineStr">
         <is>
           <t>Tahiti, French Polynesia</t>
         </is>
       </c>
-      <c r="C310" t="inlineStr">
+      <c r="C311" t="inlineStr">
         <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="D310" t="n">
+      <c r="D311" t="n">
         <v>-17.5536994934</v>
       </c>
-      <c r="E310" t="n">
+      <c r="E311" t="n">
         <v>-149.606994629</v>
       </c>
-      <c r="F310" t="inlineStr">
+      <c r="F311" t="inlineStr">
         <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="G310" t="inlineStr">
+      <c r="G311" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="H310" t="inlineStr">
+      <c r="H311" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 1112a1ee932f4aeb07a4ebf731c3b96be8f15c71
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -4102,12 +4102,12 @@
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>CZX</t>
+          <t>WUX</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Changzhou, China</t>
+          <t>Wuxi, China</t>
         </is>
       </c>
       <c r="C110" t="inlineStr"/>
@@ -4120,12 +4120,12 @@
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>WUX</t>
+          <t>YNJ</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Wuxi, China</t>
+          <t>Yanbian, China</t>
         </is>
       </c>
       <c r="C111" t="inlineStr"/>
@@ -4138,12 +4138,12 @@
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>YNJ</t>
+          <t>HGH</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Yanbian, China</t>
+          <t>Shaoxing, China</t>
         </is>
       </c>
       <c r="C112" t="inlineStr"/>
@@ -4156,46 +4156,66 @@
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>HGH</t>
+          <t>AMS</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Shaoxing, China</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr"/>
-      <c r="D113" t="inlineStr"/>
-      <c r="E113" t="inlineStr"/>
-      <c r="F113" t="inlineStr"/>
-      <c r="G113" t="inlineStr"/>
-      <c r="H113" t="inlineStr"/>
+          <t>Amsterdam, Netherlands</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>AMS</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>52.3086013794</v>
+      </c>
+      <c r="E113" t="n">
+        <v>4.7638897896</v>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>Amsterdam</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>AMS</t>
+          <t>ATH</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Amsterdam, Netherlands</t>
+          <t>Athens, Greece</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>AMS</t>
+          <t>ATH</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>52.3086013794</v>
+        <v>37.9364013672</v>
       </c>
       <c r="E114" t="n">
-        <v>4.7638897896</v>
+        <v>23.9444999695</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>GR</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
@@ -4205,35 +4225,35 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>Amsterdam</t>
+          <t>Athens</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>ATH</t>
+          <t>BCN</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Athens, Greece</t>
+          <t>Barcelona, Spain</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>ATH</t>
+          <t>BCN</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>37.9364013672</v>
+        <v>41.2971000671</v>
       </c>
       <c r="E115" t="n">
-        <v>23.9444999695</v>
+        <v>2.0784599781</v>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>GR</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
@@ -4243,35 +4263,35 @@
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>Athens</t>
+          <t>Barcelona</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>BCN</t>
+          <t>BEG</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Barcelona, Spain</t>
+          <t>Belgrade, Serbia</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>BCN</t>
+          <t>BEG</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>41.2971000671</v>
+        <v>44.8184013367</v>
       </c>
       <c r="E116" t="n">
-        <v>2.0784599781</v>
+        <v>20.3090991974</v>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>ES</t>
+          <t>RS</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
@@ -4281,35 +4301,35 @@
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>Barcelona</t>
+          <t>Belgrade</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>BEG</t>
+          <t>TXL</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Belgrade, Serbia</t>
+          <t>Berlin, Germany</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>BEG</t>
+          <t>TXL</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>44.8184013367</v>
+        <v>52.5597000122</v>
       </c>
       <c r="E117" t="n">
-        <v>20.3090991974</v>
+        <v>13.2876996994</v>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>RS</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
@@ -4319,35 +4339,35 @@
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>Belgrade</t>
+          <t>Berlin</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>TXL</t>
+          <t>BTS</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Berlin, Germany</t>
+          <t>Bratislava, Slovakia</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>TXL</t>
+          <t>BTS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>52.5597000122</v>
+        <v>48.1486</v>
       </c>
       <c r="E118" t="n">
-        <v>13.2876996994</v>
+        <v>17.1077</v>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>SK</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
@@ -4357,35 +4377,35 @@
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>Berlin</t>
+          <t>Bratislava</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>BTS</t>
+          <t>BRU</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Bratislava, Slovakia</t>
+          <t>Brussels, Belgium</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>BTS</t>
+          <t>BRU</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>48.1486</v>
+        <v>50.9014015198</v>
       </c>
       <c r="E119" t="n">
-        <v>17.1077</v>
+        <v>4.4844398499</v>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>SK</t>
+          <t>BE</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
@@ -4395,35 +4415,35 @@
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>Bratislava</t>
+          <t>Brussels</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>BRU</t>
+          <t>OTP</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Brussels, Belgium</t>
+          <t>Bucharest, Romania</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>BRU</t>
+          <t>OTP</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>50.9014015198</v>
+        <v>44.5722007751</v>
       </c>
       <c r="E120" t="n">
-        <v>4.4844398499</v>
+        <v>26.1021995544</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>BE</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
@@ -4433,35 +4453,35 @@
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>Brussels</t>
+          <t>Bucharest</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>OTP</t>
+          <t>BUD</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Bucharest, Romania</t>
+          <t>Budapest, Hungary</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>OTP</t>
+          <t>BUD</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>44.5722007751</v>
+        <v>47.4369010925</v>
       </c>
       <c r="E121" t="n">
-        <v>26.1021995544</v>
+        <v>19.2555999756</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>HU</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
@@ -4471,35 +4491,35 @@
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>Bucharest</t>
+          <t>Budapest</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>BUD</t>
+          <t>KIV</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Budapest, Hungary</t>
+          <t>Chișinău, Moldova</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>BUD</t>
+          <t>KIV</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>47.4369010925</v>
+        <v>46.9277000427</v>
       </c>
       <c r="E122" t="n">
-        <v>19.2555999756</v>
+        <v>28.9309997559</v>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>HU</t>
+          <t>MD</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
@@ -4509,35 +4529,35 @@
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>Budapest</t>
+          <t>Chișinău</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>KIV</t>
+          <t>CPH</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Chișinău, Moldova</t>
+          <t>Copenhagen, Denmark</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>KIV</t>
+          <t>CPH</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>46.9277000427</v>
+        <v>55.6179008484</v>
       </c>
       <c r="E123" t="n">
-        <v>28.9309997559</v>
+        <v>12.6560001373</v>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>MD</t>
+          <t>DK</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
@@ -4547,35 +4567,35 @@
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>Chișinău</t>
+          <t>Copenhagen</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>CPH</t>
+          <t>ORK</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Copenhagen, Denmark</t>
+          <t>Cork, Ireland</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>CPH</t>
+          <t>ORK</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>55.6179008484</v>
+        <v>51.8413009644</v>
       </c>
       <c r="E124" t="n">
-        <v>12.6560001373</v>
+        <v>-8.491109848000001</v>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>DK</t>
+          <t>IE</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
@@ -4585,31 +4605,31 @@
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>Copenhagen</t>
+          <t>Cork</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>ORK</t>
+          <t>DUB</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Cork, Ireland</t>
+          <t>Dublin, Ireland</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>ORK</t>
+          <t>DUB</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>51.8413009644</v>
+        <v>53.4212989807</v>
       </c>
       <c r="E125" t="n">
-        <v>-8.491109848000001</v>
+        <v>-6.270070076</v>
       </c>
       <c r="F125" t="inlineStr">
         <is>
@@ -4623,35 +4643,35 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>Cork</t>
+          <t>Dublin</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>DUB</t>
+          <t>DUS</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Dublin, Ireland</t>
+          <t>Düsseldorf, Germany</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>DUB</t>
+          <t>DUS</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>53.4212989807</v>
+        <v>51.2895011902</v>
       </c>
       <c r="E126" t="n">
-        <v>-6.270070076</v>
+        <v>6.7667798996</v>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
@@ -4661,35 +4681,35 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>Dublin</t>
+          <t>Düsseldorf</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>DUS</t>
+          <t>EDI</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Düsseldorf, Germany</t>
+          <t>Edinburgh, United Kingdom</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>DUS</t>
+          <t>EDI</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>51.2895011902</v>
+        <v>55.9500007629</v>
       </c>
       <c r="E127" t="n">
-        <v>6.7667798996</v>
+        <v>-3.3724999428</v>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>GB</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
@@ -4699,35 +4719,35 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>Düsseldorf</t>
+          <t>Edinburgh</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>EDI</t>
+          <t>FRA</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Edinburgh, United Kingdom</t>
+          <t>Frankfurt, Germany</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>EDI</t>
+          <t>FRA</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>55.9500007629</v>
+        <v>50.0264015198</v>
       </c>
       <c r="E128" t="n">
-        <v>-3.3724999428</v>
+        <v>8.543129921</v>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>GB</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
@@ -4737,35 +4757,35 @@
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>Edinburgh</t>
+          <t>Frankfurt</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>FRA</t>
+          <t>GVA</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Frankfurt, Germany</t>
+          <t>Geneva, Switzerland</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>FRA</t>
+          <t>GVA</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>50.0264015198</v>
+        <v>46.2380981445</v>
       </c>
       <c r="E129" t="n">
-        <v>8.543129921</v>
+        <v>6.1089501381</v>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>CH</t>
         </is>
       </c>
       <c r="G129" t="inlineStr">
@@ -4775,35 +4795,35 @@
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>Frankfurt</t>
+          <t>Geneva</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
-          <t>GVA</t>
+          <t>GOT</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Geneva, Switzerland</t>
+          <t>Gothenburg, Sweden</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>GVA</t>
+          <t>GOT</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>46.2380981445</v>
+        <v>57.6627998352</v>
       </c>
       <c r="E130" t="n">
-        <v>6.1089501381</v>
+        <v>12.279800415</v>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>CH</t>
+          <t>SE</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
@@ -4813,35 +4833,35 @@
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>Geneva</t>
+          <t>Gothenburg</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
-          <t>GOT</t>
+          <t>HAM</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Gothenburg, Sweden</t>
+          <t>Hamburg, Germany</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>GOT</t>
+          <t>HAM</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>57.6627998352</v>
+        <v>53.6304016113</v>
       </c>
       <c r="E131" t="n">
-        <v>12.279800415</v>
+        <v>9.9882297516</v>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>SE</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
@@ -4851,35 +4871,35 @@
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>Gothenburg</t>
+          <t>Hamburg</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>HAM</t>
+          <t>HEL</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Hamburg, Germany</t>
+          <t>Helsinki, Finland</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>HAM</t>
+          <t>HEL</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>53.6304016113</v>
+        <v>60.317199707</v>
       </c>
       <c r="E132" t="n">
-        <v>9.9882297516</v>
+        <v>24.963300705</v>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>FI</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
@@ -4889,35 +4909,35 @@
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>Hamburg</t>
+          <t>Helsinki</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>HEL</t>
+          <t>IST</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Helsinki, Finland</t>
+          <t>Istanbul, Turkey</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>HEL</t>
+          <t>IST</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>60.317199707</v>
+        <v>40.9768981934</v>
       </c>
       <c r="E133" t="n">
-        <v>24.963300705</v>
+        <v>28.8145999908</v>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>FI</t>
+          <t>TR</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
@@ -4927,31 +4947,31 @@
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>Helsinki</t>
+          <t>Istanbul</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>IST</t>
+          <t>ADB</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Istanbul, Turkey</t>
+          <t>Izmir, Turkey</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>IST</t>
+          <t>ADB</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>40.9768981934</v>
+        <v>38.32377</v>
       </c>
       <c r="E134" t="n">
-        <v>28.8145999908</v>
+        <v>27.14317</v>
       </c>
       <c r="F134" t="inlineStr">
         <is>
@@ -4965,35 +4985,35 @@
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Istanbul</t>
+          <t>Izmir</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
-          <t>ADB</t>
+          <t>KBP</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Izmir, Turkey</t>
+          <t>Kyiv, Ukraine</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>ADB</t>
+          <t>KBP</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>38.32377</v>
+        <v>50.3450012207</v>
       </c>
       <c r="E135" t="n">
-        <v>27.14317</v>
+        <v>30.8946990967</v>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>TR</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
@@ -5003,35 +5023,35 @@
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>Izmir</t>
+          <t>Kyiv</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
         <is>
-          <t>KBP</t>
+          <t>LIS</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Kyiv, Ukraine</t>
+          <t>Lisbon, Portugal</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>KBP</t>
+          <t>LIS</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>50.3450012207</v>
+        <v>38.7812995911</v>
       </c>
       <c r="E136" t="n">
-        <v>30.8946990967</v>
+        <v>-9.135919570900001</v>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>UA</t>
+          <t>PT</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
@@ -5041,35 +5061,35 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Kyiv</t>
+          <t>Lisbon</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>LIS</t>
+          <t>LHR</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Lisbon, Portugal</t>
+          <t>London, United Kingdom</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>LIS</t>
+          <t>LHR</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>38.7812995911</v>
+        <v>51.4706001282</v>
       </c>
       <c r="E137" t="n">
-        <v>-9.135919570900001</v>
+        <v>-0.4619410038</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>GB</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
@@ -5079,35 +5099,35 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>Lisbon</t>
+          <t>London</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>LHR</t>
+          <t>LUX</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>London, United Kingdom</t>
+          <t>Luxembourg City, Luxembourg</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>LHR</t>
+          <t>LUX</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>51.4706001282</v>
+        <v>49.6265983582</v>
       </c>
       <c r="E138" t="n">
-        <v>-0.4619410038</v>
+        <v>6.211520195</v>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>GB</t>
+          <t>LU</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
@@ -5117,35 +5137,35 @@
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>London</t>
+          <t>Luxembourg City</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>LUX</t>
+          <t>MAD</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Luxembourg City, Luxembourg</t>
+          <t>Madrid, Spain</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>LUX</t>
+          <t>MAD</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>49.6265983582</v>
+        <v>40.4936</v>
       </c>
       <c r="E139" t="n">
-        <v>6.211520195</v>
+        <v>-3.56676</v>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>LU</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
@@ -5155,35 +5175,35 @@
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>Luxembourg City</t>
+          <t>Madrid</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>MAD</t>
+          <t>MAN</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Madrid, Spain</t>
+          <t>Manchester, United Kingdom</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>MAD</t>
+          <t>MAN</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>40.4936</v>
+        <v>53.3536987305</v>
       </c>
       <c r="E140" t="n">
-        <v>-3.56676</v>
+        <v>-2.2749500275</v>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>ES</t>
+          <t>GB</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
@@ -5193,35 +5213,35 @@
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>Manchester</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>MAN</t>
+          <t>MRS</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Manchester, United Kingdom</t>
+          <t>Marseille, France</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>MAN</t>
+          <t>MRS</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>53.3536987305</v>
+        <v>43.439271922</v>
       </c>
       <c r="E141" t="n">
-        <v>-2.2749500275</v>
+        <v>5.2214241028</v>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>GB</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="G141" t="inlineStr">
@@ -5231,35 +5251,35 @@
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>Manchester</t>
+          <t>Marseille</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>MRS</t>
+          <t>MXP</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Marseille, France</t>
+          <t>Milan, Italy</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>MRS</t>
+          <t>MXP</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>43.439271922</v>
+        <v>45.6305999756</v>
       </c>
       <c r="E142" t="n">
-        <v>5.2214241028</v>
+        <v>8.7281103134</v>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
@@ -5269,35 +5289,35 @@
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>Marseille</t>
+          <t>Milan</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>MXP</t>
+          <t>MSQ</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Milan, Italy</t>
+          <t>Minsk, Belarus</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>MXP</t>
+          <t>MSQ</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>45.6305999756</v>
+        <v>53.9006</v>
       </c>
       <c r="E143" t="n">
-        <v>8.7281103134</v>
+        <v>27.599</v>
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>BY</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
@@ -5307,35 +5327,35 @@
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>Milan</t>
+          <t>Minsk</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>MSQ</t>
+          <t>DME</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Minsk, Belarus</t>
+          <t>Moscow, Russia</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>MSQ</t>
+          <t>DME</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>53.9006</v>
+        <v>55.4087982178</v>
       </c>
       <c r="E144" t="n">
-        <v>27.599</v>
+        <v>37.9062995911</v>
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>BY</t>
+          <t>RU</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
@@ -5345,35 +5365,35 @@
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>Minsk</t>
+          <t>Moscow</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>DME</t>
+          <t>MUC</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Moscow, Russia</t>
+          <t>Munich, Germany</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>DME</t>
+          <t>MUC</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>55.4087982178</v>
+        <v>48.3538017273</v>
       </c>
       <c r="E145" t="n">
-        <v>37.9062995911</v>
+        <v>11.7861003876</v>
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>RU</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
@@ -5383,35 +5403,35 @@
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t>Moscow</t>
+          <t>Munich</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>MUC</t>
+          <t>LCA</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Munich, Germany</t>
+          <t>Nicosia, Cyprus</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>MUC</t>
+          <t>LCA</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>48.3538017273</v>
+        <v>34.8750991821</v>
       </c>
       <c r="E146" t="n">
-        <v>11.7861003876</v>
+        <v>33.6249008179</v>
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>CY</t>
         </is>
       </c>
       <c r="G146" t="inlineStr">
@@ -5421,35 +5441,35 @@
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>Munich</t>
+          <t>Nicosia</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>LCA</t>
+          <t>OSL</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Nicosia, Cyprus</t>
+          <t>Oslo, Norway</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>LCA</t>
+          <t>OSL</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>34.8750991821</v>
+        <v>60.193901062</v>
       </c>
       <c r="E147" t="n">
-        <v>33.6249008179</v>
+        <v>11.100399971</v>
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>CY</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="G147" t="inlineStr">
@@ -5459,35 +5479,35 @@
       </c>
       <c r="H147" t="inlineStr">
         <is>
-          <t>Nicosia</t>
+          <t>Oslo</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
         <is>
-          <t>OSL</t>
+          <t>PMO</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Oslo, Norway</t>
+          <t>Palermo, Italy</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>OSL</t>
+          <t>PMO</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>60.193901062</v>
+        <v>38.16114</v>
       </c>
       <c r="E148" t="n">
-        <v>11.100399971</v>
+        <v>13.31546</v>
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="G148" t="inlineStr">
@@ -5497,35 +5517,35 @@
       </c>
       <c r="H148" t="inlineStr">
         <is>
-          <t>Oslo</t>
+          <t>Palermo</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>PMO</t>
+          <t>CDG</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Palermo, Italy</t>
+          <t>Paris, France</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>PMO</t>
+          <t>CDG</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>38.16114</v>
+        <v>49.0127983093</v>
       </c>
       <c r="E149" t="n">
-        <v>13.31546</v>
+        <v>2.5499999523</v>
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="G149" t="inlineStr">
@@ -5535,35 +5555,35 @@
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paris</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="inlineStr">
         <is>
-          <t>CDG</t>
+          <t>PRG</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Paris, France</t>
+          <t>Prague, Czech Republic</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>CDG</t>
+          <t>PRG</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>49.0127983093</v>
+        <v>50.1007995605</v>
       </c>
       <c r="E150" t="n">
-        <v>2.5499999523</v>
+        <v>14.2600002289</v>
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>CZ</t>
         </is>
       </c>
       <c r="G150" t="inlineStr">
@@ -5573,35 +5593,35 @@
       </c>
       <c r="H150" t="inlineStr">
         <is>
-          <t>Paris</t>
+          <t>Prague</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>PRG</t>
+          <t>KEF</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Prague, Czech Republic</t>
+          <t>Reykjavík, Iceland</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>PRG</t>
+          <t>KEF</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>50.1007995605</v>
+        <v>63.9850006104</v>
       </c>
       <c r="E151" t="n">
-        <v>14.2600002289</v>
+        <v>-22.6056003571</v>
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>CZ</t>
+          <t>IS</t>
         </is>
       </c>
       <c r="G151" t="inlineStr">
@@ -5611,35 +5631,35 @@
       </c>
       <c r="H151" t="inlineStr">
         <is>
-          <t>Prague</t>
+          <t>Reykjavík</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
         <is>
-          <t>KEF</t>
+          <t>RIX</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Reykjavík, Iceland</t>
+          <t>Riga, Latvia</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>KEF</t>
+          <t>RIX</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>63.9850006104</v>
+        <v>56.9235992432</v>
       </c>
       <c r="E152" t="n">
-        <v>-22.6056003571</v>
+        <v>23.9710998535</v>
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>IS</t>
+          <t>LV</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
@@ -5649,35 +5669,35 @@
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>Reykjavík</t>
+          <t>Riga</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
-          <t>RIX</t>
+          <t>FCO</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Riga, Latvia</t>
+          <t>Rome, Italy</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>RIX</t>
+          <t>FCO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>56.9235992432</v>
+        <v>41.8045005798</v>
       </c>
       <c r="E153" t="n">
-        <v>23.9710998535</v>
+        <v>12.2508001328</v>
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>LV</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="G153" t="inlineStr">
@@ -5687,35 +5707,35 @@
       </c>
       <c r="H153" t="inlineStr">
         <is>
-          <t>Riga</t>
+          <t>Rome</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="inlineStr">
         <is>
-          <t>FCO</t>
+          <t>LED</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Rome, Italy</t>
+          <t>Saint Petersburg, Russia</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>FCO</t>
+          <t>LED</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>41.8045005798</v>
+        <v>59.8003005981</v>
       </c>
       <c r="E154" t="n">
-        <v>12.2508001328</v>
+        <v>30.2625007629</v>
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>RU</t>
         </is>
       </c>
       <c r="G154" t="inlineStr">
@@ -5725,35 +5745,35 @@
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>Rome</t>
+          <t>Saint Petersburg</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="inlineStr">
         <is>
-          <t>LED</t>
+          <t>SOF</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Saint Petersburg, Russia</t>
+          <t>Sofia, Bulgaria</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>LED</t>
+          <t>SOF</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>59.8003005981</v>
+        <v>42.6966934204</v>
       </c>
       <c r="E155" t="n">
-        <v>30.2625007629</v>
+        <v>23.4114360809</v>
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>RU</t>
+          <t>BG</t>
         </is>
       </c>
       <c r="G155" t="inlineStr">
@@ -5763,35 +5783,35 @@
       </c>
       <c r="H155" t="inlineStr">
         <is>
-          <t>Saint Petersburg</t>
+          <t>Sofia</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="inlineStr">
         <is>
-          <t>SOF</t>
+          <t>ARN</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Sofia, Bulgaria</t>
+          <t>Stockholm, Sweden</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>SOF</t>
+          <t>ARN</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>42.6966934204</v>
+        <v>59.6519012451</v>
       </c>
       <c r="E156" t="n">
-        <v>23.4114360809</v>
+        <v>17.9186000824</v>
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>BG</t>
+          <t>SE</t>
         </is>
       </c>
       <c r="G156" t="inlineStr">
@@ -5801,35 +5821,35 @@
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>Sofia</t>
+          <t>Stockholm</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="inlineStr">
         <is>
-          <t>ARN</t>
+          <t>STR</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Stockholm, Sweden</t>
+          <t>Stuttgart, Germany</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>ARN</t>
+          <t>STR</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>59.6519012451</v>
+        <v>48.783333</v>
       </c>
       <c r="E157" t="n">
-        <v>17.9186000824</v>
+        <v>9.183332999999999</v>
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>SE</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="G157" t="inlineStr">
@@ -5839,35 +5859,35 @@
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>Stockholm</t>
+          <t>Stuttgart</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="inlineStr">
         <is>
-          <t>STR</t>
+          <t>TLL</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Stuttgart, Germany</t>
+          <t>Tallinn, Estonia</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>STR</t>
+          <t>TLL</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>48.783333</v>
+        <v>59.4132995605</v>
       </c>
       <c r="E158" t="n">
-        <v>9.183332999999999</v>
+        <v>24.8327999115</v>
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>EE</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
@@ -5877,35 +5897,35 @@
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>Stuttgart</t>
+          <t>Tallinn</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
         <is>
-          <t>TLL</t>
+          <t>TBS</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Tallinn, Estonia</t>
+          <t>Tbilisi, Georgia</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>TLL</t>
+          <t>TBS</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>59.4132995605</v>
+        <v>41.6692008972</v>
       </c>
       <c r="E159" t="n">
-        <v>24.8327999115</v>
+        <v>44.95470047</v>
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>EE</t>
+          <t>GE</t>
         </is>
       </c>
       <c r="G159" t="inlineStr">
@@ -5915,35 +5935,35 @@
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>Tallinn</t>
+          <t>Tbilisi</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
         <is>
-          <t>TBS</t>
+          <t>SKG</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Tbilisi, Georgia</t>
+          <t>Thessaloniki, Greece</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>TBS</t>
+          <t>SKG</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>41.6692008972</v>
+        <v>40.5196990967</v>
       </c>
       <c r="E160" t="n">
-        <v>44.95470047</v>
+        <v>22.9708995819</v>
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>GE</t>
+          <t>GR</t>
         </is>
       </c>
       <c r="G160" t="inlineStr">
@@ -5953,35 +5973,35 @@
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>Tbilisi</t>
+          <t>Thessaloniki</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
-          <t>SKG</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Thessaloniki, Greece</t>
+          <t>Tirana, Albania</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>SKG</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>40.5196990967</v>
+        <v>41.4146995544</v>
       </c>
       <c r="E161" t="n">
-        <v>22.9708995819</v>
+        <v>19.7206001282</v>
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>GR</t>
+          <t>AL</t>
         </is>
       </c>
       <c r="G161" t="inlineStr">
@@ -5991,35 +6011,35 @@
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>Thessaloniki</t>
+          <t>Tirana</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>KLD</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Tirana, Albania</t>
+          <t>Tver, Russian Federation</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>KLD</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>41.4146995544</v>
+        <v>56.8587</v>
       </c>
       <c r="E162" t="n">
-        <v>19.7206001282</v>
+        <v>35.9176</v>
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>AL</t>
+          <t>RU</t>
         </is>
       </c>
       <c r="G162" t="inlineStr">
@@ -6029,35 +6049,35 @@
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>Tirana</t>
+          <t>Tver</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="inlineStr">
         <is>
-          <t>KLD</t>
+          <t>VIE</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Tver, Russian Federation</t>
+          <t>Vienna, Austria</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>KLD</t>
+          <t>VIE</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>56.8587</v>
+        <v>48.1102981567</v>
       </c>
       <c r="E163" t="n">
-        <v>35.9176</v>
+        <v>16.5697002411</v>
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>RU</t>
+          <t>AT</t>
         </is>
       </c>
       <c r="G163" t="inlineStr">
@@ -6067,35 +6087,35 @@
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>Tver</t>
+          <t>Vienna</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
         <is>
-          <t>VIE</t>
+          <t>VNO</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Vienna, Austria</t>
+          <t>Vilnius, Lithuania</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>VIE</t>
+          <t>VNO</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>48.1102981567</v>
+        <v>54.6341018677</v>
       </c>
       <c r="E164" t="n">
-        <v>16.5697002411</v>
+        <v>25.2858009338</v>
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>AT</t>
+          <t>LT</t>
         </is>
       </c>
       <c r="G164" t="inlineStr">
@@ -6105,35 +6125,35 @@
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>Vienna</t>
+          <t>Vilnius</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>VNO</t>
+          <t>WAW</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Vilnius, Lithuania</t>
+          <t>Warsaw, Poland</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>VNO</t>
+          <t>WAW</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>54.6341018677</v>
+        <v>52.1656990051</v>
       </c>
       <c r="E165" t="n">
-        <v>25.2858009338</v>
+        <v>20.9671001434</v>
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>LT</t>
+          <t>PL</t>
         </is>
       </c>
       <c r="G165" t="inlineStr">
@@ -6143,111 +6163,111 @@
       </c>
       <c r="H165" t="inlineStr">
         <is>
-          <t>Vilnius</t>
+          <t>Warsaw</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>WAW</t>
+          <t>SVX</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Warsaw, Poland</t>
+          <t>Yekaterinburg, Russia</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>WAW</t>
+          <t>SVX</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>52.1656990051</v>
+        <v>56.8431</v>
       </c>
       <c r="E166" t="n">
-        <v>20.9671001434</v>
+        <v>60.6454</v>
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>PL</t>
+          <t>RU</t>
         </is>
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>Warsaw</t>
+          <t>Yekaterinburg</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>SVX</t>
+          <t>ZAG</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Yekaterinburg, Russia</t>
+          <t>Zagreb, Croatia</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>SVX</t>
+          <t>ZAG</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>56.8431</v>
+        <v>45.7429008484</v>
       </c>
       <c r="E167" t="n">
-        <v>60.6454</v>
+        <v>16.0687999725</v>
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>RU</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>Yekaterinburg</t>
+          <t>Zagreb</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>ZAG</t>
+          <t>ZRH</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Zagreb, Croatia</t>
+          <t>Zürich, Switzerland</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>ZAG</t>
+          <t>ZRH</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>45.7429008484</v>
+        <v>47.4646987915</v>
       </c>
       <c r="E168" t="n">
-        <v>16.0687999725</v>
+        <v>8.549169540399999</v>
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>CH</t>
         </is>
       </c>
       <c r="G168" t="inlineStr">
@@ -6257,35 +6277,35 @@
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>Zagreb</t>
+          <t>Zurich</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>ZRH</t>
+          <t>LYS</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Zürich, Switzerland</t>
+          <t>Lyon, France</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>ZRH</t>
+          <t>LYS</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>47.4646987915</v>
+        <v>45.7263</v>
       </c>
       <c r="E169" t="n">
-        <v>8.549169540399999</v>
+        <v>5.0908</v>
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>CH</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="G169" t="inlineStr">
@@ -6295,31 +6315,31 @@
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>Zurich</t>
+          <t>Lyon</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>LYS</t>
+          <t>BOD</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Lyon, France</t>
+          <t>Bordeaux, France</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>LYS</t>
+          <t>BOD</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>45.7263</v>
+        <v>44.82946</v>
       </c>
       <c r="E170" t="n">
-        <v>5.0908</v>
+        <v>-0.58355</v>
       </c>
       <c r="F170" t="inlineStr">
         <is>
@@ -6333,73 +6353,73 @@
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>Lyon</t>
+          <t>Bordeaux</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>BOD</t>
+          <t>QWJ</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Bordeaux, France</t>
+          <t>Americana, Brazil</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>BOD</t>
+          <t>QWJ</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>44.82946</v>
+        <v>-22.738</v>
       </c>
       <c r="E171" t="n">
-        <v>-0.58355</v>
+        <v>-47.334</v>
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>Bordeaux</t>
+          <t>Americana</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>QWJ</t>
+          <t>ARI</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Americana, Brazil</t>
+          <t>Arica, Chile</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>QWJ</t>
+          <t>ARI</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>-22.738</v>
+        <v>-18.348611</v>
       </c>
       <c r="E172" t="n">
-        <v>-47.334</v>
+        <v>-70.33888899999999</v>
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="G172" t="inlineStr">
@@ -6409,35 +6429,35 @@
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>Americana</t>
+          <t>Arica</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>ARI</t>
+          <t>ASU</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Arica, Chile</t>
+          <t>Asunción, Paraguay</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>ARI</t>
+          <t>ASU</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>-18.348611</v>
+        <v>-25.2399997711</v>
       </c>
       <c r="E173" t="n">
-        <v>-70.33888899999999</v>
+        <v>-57.5200004578</v>
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>PY</t>
         </is>
       </c>
       <c r="G173" t="inlineStr">
@@ -6447,35 +6467,35 @@
       </c>
       <c r="H173" t="inlineStr">
         <is>
-          <t>Arica</t>
+          <t>Asunción</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>ASU</t>
+          <t>BEL</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Asunción, Paraguay</t>
+          <t>Belém, Brazil</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>ASU</t>
+          <t>BEL</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>-25.2399997711</v>
+        <v>-1.4563</v>
       </c>
       <c r="E174" t="n">
-        <v>-57.5200004578</v>
+        <v>-48.5013</v>
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>PY</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G174" t="inlineStr">
@@ -6485,31 +6505,31 @@
       </c>
       <c r="H174" t="inlineStr">
         <is>
-          <t>Asunción</t>
+          <t>Belém</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>BEL</t>
+          <t>CNF</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Belém, Brazil</t>
+          <t>Belo Horizonte, Brazil</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>BEL</t>
+          <t>CNF</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>-1.4563</v>
+        <v>-19.624444</v>
       </c>
       <c r="E175" t="n">
-        <v>-48.5013</v>
+        <v>-43.971944</v>
       </c>
       <c r="F175" t="inlineStr">
         <is>
@@ -6523,31 +6543,31 @@
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>Belém</t>
+          <t>Belo Horizonte</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>CNF</t>
+          <t>BNU</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Belo Horizonte, Brazil</t>
+          <t>Blumenau, Brazil</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>CNF</t>
+          <t>BNU</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>-19.624444</v>
+        <v>-26.89245</v>
       </c>
       <c r="E176" t="n">
-        <v>-43.971944</v>
+        <v>-49.07696</v>
       </c>
       <c r="F176" t="inlineStr">
         <is>
@@ -6561,35 +6581,35 @@
       </c>
       <c r="H176" t="inlineStr">
         <is>
-          <t>Belo Horizonte</t>
+          <t>Blumenau</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>BNU</t>
+          <t>BOG</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Blumenau, Brazil</t>
+          <t>Bogotá, Colombia</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>BNU</t>
+          <t>BOG</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>-26.89245</v>
+        <v>4.70159</v>
       </c>
       <c r="E177" t="n">
-        <v>-49.07696</v>
+        <v>-74.1469</v>
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="G177" t="inlineStr">
@@ -6599,35 +6619,35 @@
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>Blumenau</t>
+          <t>Bogotá</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>BOG</t>
+          <t>BSB</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Bogotá, Colombia</t>
+          <t>Brasilia, Brazil</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>BOG</t>
+          <t>BSB</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>4.70159</v>
+        <v>-15.79824</v>
       </c>
       <c r="E178" t="n">
-        <v>-74.1469</v>
+        <v>-47.90859</v>
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G178" t="inlineStr">
@@ -6637,35 +6657,35 @@
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>BSB</t>
+          <t>EZE</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Brasilia, Brazil</t>
+          <t>Buenos Aires, Argentina</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>BSB</t>
+          <t>EZE</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>-15.79824</v>
+        <v>-34.8222</v>
       </c>
       <c r="E179" t="n">
-        <v>-47.90859</v>
+        <v>-58.5358</v>
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="G179" t="inlineStr">
@@ -6675,35 +6695,35 @@
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>Brasilia</t>
+          <t>Buenos Aires</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>EZE</t>
+          <t>CFC</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Buenos Aires, Argentina</t>
+          <t>Caçador, Brazil</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>EZE</t>
+          <t>CFC</t>
         </is>
       </c>
       <c r="D180" t="n">
-        <v>-34.8222</v>
+        <v>-26.7762</v>
       </c>
       <c r="E180" t="n">
-        <v>-58.5358</v>
+        <v>-51.0125</v>
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G180" t="inlineStr">
@@ -6713,31 +6733,31 @@
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>Buenos Aires</t>
+          <t>Cacador</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>CFC</t>
+          <t>VCP</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Caçador, Brazil</t>
+          <t>Campinas, Brazil</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>CFC</t>
+          <t>VCP</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>-26.7762</v>
+        <v>-22.90662</v>
       </c>
       <c r="E181" t="n">
-        <v>-51.0125</v>
+        <v>-47.08576</v>
       </c>
       <c r="F181" t="inlineStr">
         <is>
@@ -6751,35 +6771,35 @@
       </c>
       <c r="H181" t="inlineStr">
         <is>
-          <t>Cacador</t>
+          <t>Campinas</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>VCP</t>
+          <t>COR</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Campinas, Brazil</t>
+          <t>Córdoba, Argentina</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>VCP</t>
+          <t>COR</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>-22.90662</v>
+        <v>-31.31</v>
       </c>
       <c r="E182" t="n">
-        <v>-47.08576</v>
+        <v>-64.208333</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="G182" t="inlineStr">
@@ -6789,35 +6809,35 @@
       </c>
       <c r="H182" t="inlineStr">
         <is>
-          <t>Campinas</t>
+          <t>Córdoba</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>COR</t>
+          <t>CGB</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Córdoba, Argentina</t>
+          <t>Cuiabá, Brazil</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>COR</t>
+          <t>CGB</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>-31.31</v>
+        <v>-15.59611</v>
       </c>
       <c r="E183" t="n">
-        <v>-64.208333</v>
+        <v>-56.09667</v>
       </c>
       <c r="F183" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G183" t="inlineStr">
@@ -6827,31 +6847,31 @@
       </c>
       <c r="H183" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Cuiaba</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>CGB</t>
+          <t>CWB</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Cuiabá, Brazil</t>
+          <t>Curitiba, Brazil</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>CGB</t>
+          <t>CWB</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>-15.59611</v>
+        <v>-25.5284996033</v>
       </c>
       <c r="E184" t="n">
-        <v>-56.09667</v>
+        <v>-49.1758003235</v>
       </c>
       <c r="F184" t="inlineStr">
         <is>
@@ -6865,31 +6885,31 @@
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>Cuiaba</t>
+          <t>Curitiba</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>CWB</t>
+          <t>FLN</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Curitiba, Brazil</t>
+          <t>Florianopolis, Brazil</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>CWB</t>
+          <t>FLN</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>-25.5284996033</v>
+        <v>-27.6702785492</v>
       </c>
       <c r="E185" t="n">
-        <v>-49.1758003235</v>
+        <v>-48.5525016785</v>
       </c>
       <c r="F185" t="inlineStr">
         <is>
@@ -6903,31 +6923,31 @@
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>Curitiba</t>
+          <t>Florianopolis</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>FLN</t>
+          <t>FOR</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Florianopolis, Brazil</t>
+          <t>Fortaleza, Brazil</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>FLN</t>
+          <t>FOR</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>-27.6702785492</v>
+        <v>-3.7762799263</v>
       </c>
       <c r="E186" t="n">
-        <v>-48.5525016785</v>
+        <v>-38.5326004028</v>
       </c>
       <c r="F186" t="inlineStr">
         <is>
@@ -6941,35 +6961,35 @@
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>Florianopolis</t>
+          <t>Fortaleza</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
         <is>
-          <t>FOR</t>
+          <t>GEO</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Fortaleza, Brazil</t>
+          <t>Georgetown, Guyana</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>FOR</t>
+          <t>GEO</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>-3.7762799263</v>
+        <v>6.825648</v>
       </c>
       <c r="E187" t="n">
-        <v>-38.5326004028</v>
+        <v>-58.163756</v>
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GY</t>
         </is>
       </c>
       <c r="G187" t="inlineStr">
@@ -6979,35 +6999,35 @@
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Georgetown</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
         <is>
-          <t>GEO</t>
+          <t>GYN</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Georgetown, Guyana</t>
+          <t>Goiânia, Brazil</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>GEO</t>
+          <t>GYN</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>6.825648</v>
+        <v>-16.69727</v>
       </c>
       <c r="E188" t="n">
-        <v>-58.163756</v>
+        <v>-49.26851</v>
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>GY</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G188" t="inlineStr">
@@ -7017,111 +7037,111 @@
       </c>
       <c r="H188" t="inlineStr">
         <is>
-          <t>Georgetown</t>
+          <t>Goiania</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>GYN</t>
+          <t>GUA</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Goiânia, Brazil</t>
+          <t>Guatemala City, Guatemala</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>GYN</t>
+          <t>GUA</t>
         </is>
       </c>
       <c r="D189" t="n">
-        <v>-16.69727</v>
+        <v>14.5832996368</v>
       </c>
       <c r="E189" t="n">
-        <v>-49.26851</v>
+        <v>-90.5274963379</v>
       </c>
       <c r="F189" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GT</t>
         </is>
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="H189" t="inlineStr">
         <is>
-          <t>Goiania</t>
+          <t>Guatemala City</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
         <is>
-          <t>GUA</t>
+          <t>GYE</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Guatemala City, Guatemala</t>
+          <t>Guayaquil, Ecuador</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>GUA</t>
+          <t>GYE</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>14.5832996368</v>
+        <v>-2.1894</v>
       </c>
       <c r="E190" t="n">
-        <v>-90.5274963379</v>
+        <v>-79.8891</v>
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t>GT</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="H190" t="inlineStr">
         <is>
-          <t>Guatemala City</t>
+          <t>Guayaquil</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
         <is>
-          <t>GYE</t>
+          <t>ITJ</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Guayaquil, Ecuador</t>
+          <t>Itajaí, Brazil</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>GYE</t>
+          <t>ITJ</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>-2.1894</v>
+        <v>-27.6116676331</v>
       </c>
       <c r="E191" t="n">
-        <v>-79.8891</v>
+        <v>-48.6727790833</v>
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G191" t="inlineStr">
@@ -7131,31 +7151,31 @@
       </c>
       <c r="H191" t="inlineStr">
         <is>
-          <t>Guayaquil</t>
+          <t>Itajai</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
         <is>
-          <t>ITJ</t>
+          <t>JOI</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Itajaí, Brazil</t>
+          <t>Joinville, Brazil</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>ITJ</t>
+          <t>JOI</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>-27.6116676331</v>
+        <v>-26.304408</v>
       </c>
       <c r="E192" t="n">
-        <v>-48.6727790833</v>
+        <v>-48.846383</v>
       </c>
       <c r="F192" t="inlineStr">
         <is>
@@ -7169,31 +7189,31 @@
       </c>
       <c r="H192" t="inlineStr">
         <is>
-          <t>Itajai</t>
+          <t>Joinville</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
         <is>
-          <t>JOI</t>
+          <t>JDO</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Joinville, Brazil</t>
+          <t>Juazeiro do Norte, Brazil</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>JOI</t>
+          <t>JDO</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>-26.304408</v>
+        <v>-7.2242</v>
       </c>
       <c r="E193" t="n">
-        <v>-48.846383</v>
+        <v>-39.313</v>
       </c>
       <c r="F193" t="inlineStr">
         <is>
@@ -7207,35 +7227,35 @@
       </c>
       <c r="H193" t="inlineStr">
         <is>
-          <t>Joinville</t>
+          <t>Juazeiro do Norte</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
         <is>
-          <t>JDO</t>
+          <t>LIM</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte, Brazil</t>
+          <t>Lima, Peru</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>JDO</t>
+          <t>LIM</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>-7.2242</v>
+        <v>-12.021900177</v>
       </c>
       <c r="E194" t="n">
-        <v>-39.313</v>
+        <v>-77.1143035889</v>
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="G194" t="inlineStr">
@@ -7245,35 +7265,35 @@
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte</t>
+          <t>Lima</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
         <is>
-          <t>LIM</t>
+          <t>MAO</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Lima, Peru</t>
+          <t>Manaus, Brazil</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>LIM</t>
+          <t>MAO</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>-12.021900177</v>
+        <v>-3.11286</v>
       </c>
       <c r="E195" t="n">
-        <v>-77.1143035889</v>
+        <v>-60.01949</v>
       </c>
       <c r="F195" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G195" t="inlineStr">
@@ -7283,35 +7303,35 @@
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>Lima</t>
+          <t>Manaus</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
         <is>
-          <t>MAO</t>
+          <t>MDE</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Manaus, Brazil</t>
+          <t>Medellín, Colombia</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>MAO</t>
+          <t>MDE</t>
         </is>
       </c>
       <c r="D196" t="n">
-        <v>-3.11286</v>
+        <v>6.16454</v>
       </c>
       <c r="E196" t="n">
-        <v>-60.01949</v>
+        <v>-75.42310000000001</v>
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="G196" t="inlineStr">
@@ -7321,35 +7341,35 @@
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>Manaus</t>
+          <t>Medellín</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>MDE</t>
+          <t>NQN</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Medellín, Colombia</t>
+          <t>Neuquén, Argentina</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>MDE</t>
+          <t>NQN</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>6.16454</v>
+        <v>-38.9490013123</v>
       </c>
       <c r="E197" t="n">
-        <v>-75.42310000000001</v>
+        <v>-68.1557006836</v>
       </c>
       <c r="F197" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="G197" t="inlineStr">
@@ -7359,35 +7379,35 @@
       </c>
       <c r="H197" t="inlineStr">
         <is>
-          <t>Medellín</t>
+          <t>Neuquen</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>NQN</t>
+          <t>PTY</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Neuquén, Argentina</t>
+          <t>Panama City, Panama</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>NQN</t>
+          <t>PTY</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>-38.9490013123</v>
+        <v>9.0713596344</v>
       </c>
       <c r="E198" t="n">
-        <v>-68.1557006836</v>
+        <v>-79.3834991455</v>
       </c>
       <c r="F198" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="G198" t="inlineStr">
@@ -7397,35 +7417,35 @@
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>Neuquen</t>
+          <t>Panama City</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>PTY</t>
+          <t>PBM</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Panama City, Panama</t>
+          <t>Paramaribo, Suriname</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>PTY</t>
+          <t>PBM</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>9.0713596344</v>
+        <v>5.452831</v>
       </c>
       <c r="E199" t="n">
-        <v>-79.3834991455</v>
+        <v>-55.187783</v>
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>SR</t>
         </is>
       </c>
       <c r="G199" t="inlineStr">
@@ -7435,35 +7455,35 @@
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>Panama City</t>
+          <t>Paramaribo</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>PBM</t>
+          <t>POA</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Paramaribo, Suriname</t>
+          <t>Porto Alegre, Brazil</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>PBM</t>
+          <t>POA</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>5.452831</v>
+        <v>-29.9944000244</v>
       </c>
       <c r="E200" t="n">
-        <v>-55.187783</v>
+        <v>-51.1713981628</v>
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>SR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G200" t="inlineStr">
@@ -7473,35 +7493,35 @@
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>Paramaribo</t>
+          <t>Porto Alegre</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>POA</t>
+          <t>UIO</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Porto Alegre, Brazil</t>
+          <t>Quito, Ecuador</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>POA</t>
+          <t>UIO</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>-29.9944000244</v>
+        <v>-0.1291666667</v>
       </c>
       <c r="E201" t="n">
-        <v>-51.1713981628</v>
+        <v>-78.3575</v>
       </c>
       <c r="F201" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="G201" t="inlineStr">
@@ -7511,35 +7531,35 @@
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>Porto Alegre</t>
+          <t>Quito</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>UIO</t>
+          <t>REC</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Quito, Ecuador</t>
+          <t>Recife, Brazil</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>UIO</t>
+          <t>REC</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>-0.1291666667</v>
+        <v>-8.126489639300001</v>
       </c>
       <c r="E202" t="n">
-        <v>-78.3575</v>
+        <v>-34.9235992432</v>
       </c>
       <c r="F202" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G202" t="inlineStr">
@@ -7549,31 +7569,31 @@
       </c>
       <c r="H202" t="inlineStr">
         <is>
-          <t>Quito</t>
+          <t>Recife</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Recife, Brazil</t>
+          <t>Ribeirao Preto, Brazil</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>-8.126489639300001</v>
+        <v>-21.1363887787</v>
       </c>
       <c r="E203" t="n">
-        <v>-34.9235992432</v>
+        <v>-47.7766685486</v>
       </c>
       <c r="F203" t="inlineStr">
         <is>
@@ -7587,31 +7607,31 @@
       </c>
       <c r="H203" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>Ribeirao Preto</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>GIG</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Ribeirao Preto, Brazil</t>
+          <t>Rio de Janeiro, Brazil</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>GIG</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>-21.1363887787</v>
+        <v>-22.8099994659</v>
       </c>
       <c r="E204" t="n">
-        <v>-47.7766685486</v>
+        <v>-43.2505569458</v>
       </c>
       <c r="F204" t="inlineStr">
         <is>
@@ -7625,31 +7645,31 @@
       </c>
       <c r="H204" t="inlineStr">
         <is>
-          <t>Ribeirao Preto</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>GIG</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Rio de Janeiro, Brazil</t>
+          <t>Salvador, Brazil</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>GIG</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="D205" t="n">
-        <v>-22.8099994659</v>
+        <v>-12.9086112976</v>
       </c>
       <c r="E205" t="n">
-        <v>-43.2505569458</v>
+        <v>-38.3224983215</v>
       </c>
       <c r="F205" t="inlineStr">
         <is>
@@ -7663,35 +7683,35 @@
       </c>
       <c r="H205" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Salvador, Brazil</t>
+          <t>San José, Costa Rica</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>-12.9086112976</v>
+        <v>9.9938602448</v>
       </c>
       <c r="E206" t="n">
-        <v>-38.3224983215</v>
+        <v>-84.2088012695</v>
       </c>
       <c r="F206" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="G206" t="inlineStr">
@@ -7701,35 +7721,35 @@
       </c>
       <c r="H206" t="inlineStr">
         <is>
-          <t>Salvador</t>
+          <t>San José</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>San José, Costa Rica</t>
+          <t>Santiago, Chile</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>9.9938602448</v>
+        <v>-33.3930015564</v>
       </c>
       <c r="E207" t="n">
-        <v>-84.2088012695</v>
+        <v>-70.7857971191</v>
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="G207" t="inlineStr">
@@ -7739,107 +7759,107 @@
       </c>
       <c r="H207" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Santiago</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SDQ</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Santiago, Chile</t>
+          <t>Santo Domingo, Dominican Republic</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SDQ</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>-33.3930015564</v>
+        <v>18.4297008514</v>
       </c>
       <c r="E208" t="n">
-        <v>-70.7857971191</v>
+        <v>-69.6688995361</v>
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>Santo Domingo</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>SDQ</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Santo Domingo, Dominican Republic</t>
+          <t>São José do Rio Preto, Brazil</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>SDQ</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>18.4297008514</v>
+        <v>-20.807157</v>
       </c>
       <c r="E209" t="n">
-        <v>-69.6688995361</v>
+        <v>-49.378994</v>
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t>DO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>Santo Domingo</t>
+          <t>São José do Rio Preto</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SJK</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>São José do Rio Preto, Brazil</t>
+          <t>São José dos Campos, Brazil</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SJK</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>-20.807157</v>
+        <v>-23.1791</v>
       </c>
       <c r="E210" t="n">
-        <v>-49.378994</v>
+        <v>-45.8872</v>
       </c>
       <c r="F210" t="inlineStr">
         <is>
@@ -7853,31 +7873,31 @@
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>São José dos Campos</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>SJK</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>São José dos Campos, Brazil</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>SJK</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>-23.1791</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="E211" t="n">
-        <v>-45.8872</v>
+        <v>-46.4730567932</v>
       </c>
       <c r="F211" t="inlineStr">
         <is>
@@ -7891,31 +7911,31 @@
       </c>
       <c r="H211" t="inlineStr">
         <is>
-          <t>São José dos Campos</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>-23.4355564117</v>
+        <v>-23.54389</v>
       </c>
       <c r="E212" t="n">
-        <v>-46.4730567932</v>
+        <v>-46.63445</v>
       </c>
       <c r="F212" t="inlineStr">
         <is>
@@ -7929,35 +7949,35 @@
       </c>
       <c r="H212" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Sorocaba</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>-23.54389</v>
+        <v>12.007116</v>
       </c>
       <c r="E213" t="n">
-        <v>-46.63445</v>
+        <v>-61.7882288</v>
       </c>
       <c r="F213" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="G213" t="inlineStr">
@@ -7967,35 +7987,35 @@
       </c>
       <c r="H213" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>12.007116</v>
+        <v>14.0608</v>
       </c>
       <c r="E214" t="n">
-        <v>-61.7882288</v>
+        <v>-87.21720000000001</v>
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="G214" t="inlineStr">
@@ -8005,35 +8025,35 @@
       </c>
       <c r="H214" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>NVT</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>Timbó, Brazil</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>NVT</t>
         </is>
       </c>
       <c r="D215" t="n">
-        <v>14.0608</v>
+        <v>-26.8251</v>
       </c>
       <c r="E215" t="n">
-        <v>-87.21720000000001</v>
+        <v>-49.2695</v>
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G215" t="inlineStr">
@@ -8043,31 +8063,31 @@
       </c>
       <c r="H215" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>Timbo</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>NVT</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Timbó, Brazil</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>NVT</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>-26.8251</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="E216" t="n">
-        <v>-49.2695</v>
+        <v>-48.225276947</v>
       </c>
       <c r="F216" t="inlineStr">
         <is>
@@ -8081,31 +8101,31 @@
       </c>
       <c r="H216" t="inlineStr">
         <is>
-          <t>Timbo</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>VIX</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Vitoria, Brazil</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>VIX</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>-18.8836116791</v>
+        <v>-20.64871</v>
       </c>
       <c r="E217" t="n">
-        <v>-48.225276947</v>
+        <v>-41.90857</v>
       </c>
       <c r="F217" t="inlineStr">
         <is>
@@ -8119,107 +8139,107 @@
       </c>
       <c r="H217" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Vitoria</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>VIX</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Vitoria, Brazil</t>
+          <t>Willemstad, Curaçao</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>VIX</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>-20.64871</v>
+        <v>12.1888999939</v>
       </c>
       <c r="E218" t="n">
-        <v>-41.90857</v>
+        <v>-68.95980072019999</v>
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="H218" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Willemstad</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>CAW</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Campos dos Goytacazes, Brazil</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>CAW</t>
         </is>
       </c>
       <c r="D219" t="n">
-        <v>12.1888999939</v>
+        <v>-21.698299408</v>
       </c>
       <c r="E219" t="n">
-        <v>-68.95980072019999</v>
+        <v>-41.301700592</v>
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="H219" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Campos dos Goytacazes</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>CAW</t>
+          <t>XAP</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes, Brazil</t>
+          <t>Chapeco, Brazil</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>CAW</t>
+          <t>XAP</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>-21.698299408</v>
+        <v>-27.1341991425</v>
       </c>
       <c r="E220" t="n">
-        <v>-41.301700592</v>
+        <v>-52.6566009521</v>
       </c>
       <c r="F220" t="inlineStr">
         <is>
@@ -8233,45 +8253,45 @@
       </c>
       <c r="H220" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes</t>
+          <t>Chapeco</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>XAP</t>
+          <t>BGI</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Chapeco, Brazil</t>
+          <t>Bridgetown, Barbados</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>XAP</t>
+          <t>BGI</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>-27.1341991425</v>
+        <v>13.103562</v>
       </c>
       <c r="E221" t="n">
-        <v>-52.6566009521</v>
+        <v>-59.603226</v>
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="H221" t="inlineStr">
         <is>
-          <t>Chapeco</t>
+          <t>Bridgetown</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by fc8c26edcc1dc4784d937bedcc772cea29511858
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H313"/>
+  <dimension ref="A1:H314"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11318,66 +11318,66 @@
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>-34.9431729</v>
+        <v>27.9755001068</v>
       </c>
       <c r="E302" t="n">
-        <v>138.5335637</v>
+        <v>-82.533203125</v>
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="H302" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="E303" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="G303" t="inlineStr">
@@ -11387,35 +11387,35 @@
       </c>
       <c r="H303" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="E304" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="G304" t="inlineStr">
@@ -11425,31 +11425,31 @@
       </c>
       <c r="H304" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="E305" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="F305" t="inlineStr">
         <is>
@@ -11463,35 +11463,35 @@
       </c>
       <c r="H305" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="E306" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="G306" t="inlineStr">
@@ -11501,107 +11501,107 @@
       </c>
       <c r="H306" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="E307" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="H307" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="E308" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="H308" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="E309" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="F309" t="inlineStr">
         <is>
@@ -11615,35 +11615,35 @@
       </c>
       <c r="H309" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="E310" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="G310" t="inlineStr">
@@ -11653,35 +11653,35 @@
       </c>
       <c r="H310" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="E311" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="G311" t="inlineStr">
@@ -11691,31 +11691,31 @@
       </c>
       <c r="H311" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="E312" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="F312" t="inlineStr">
         <is>
@@ -11729,43 +11729,81 @@
       </c>
       <c r="H312" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Sydney, NSW, Australia</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>-33.9460983276</v>
+      </c>
+      <c r="E313" t="n">
+        <v>151.177001953</v>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="G313" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="H313" t="inlineStr">
+        <is>
+          <t>Sydney</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="1" t="inlineStr">
+        <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="B313" t="inlineStr">
+      <c r="B314" t="inlineStr">
         <is>
           <t>Tahiti, French Polynesia</t>
         </is>
       </c>
-      <c r="C313" t="inlineStr">
+      <c r="C314" t="inlineStr">
         <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="D313" t="n">
+      <c r="D314" t="n">
         <v>-17.5536994934</v>
       </c>
-      <c r="E313" t="n">
+      <c r="E314" t="n">
         <v>-149.606994629</v>
       </c>
-      <c r="F313" t="inlineStr">
+      <c r="F314" t="inlineStr">
         <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="G313" t="inlineStr">
+      <c r="G314" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="H313" t="inlineStr">
+      <c r="H314" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>